<commit_message>
added time zone to date parser
</commit_message>
<xml_diff>
--- a/Feature Matrix.xlsx
+++ b/Feature Matrix.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="118">
   <si>
     <t>Feature</t>
   </si>
@@ -364,6 +364,15 @@
   <si>
     <t>copies html with color</t>
   </si>
+  <si>
+    <t>shows time zone</t>
+  </si>
+  <si>
+    <t>show tool bar</t>
+  </si>
+  <si>
+    <t>copies rtf with color</t>
+  </si>
 </sst>
 </file>
 
@@ -482,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -575,9 +584,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,7 +627,7 @@
           <c:yMode val="edge"/>
           <c:x val="3.8461559098965002E-2"/>
           <c:y val="2.2690437601296611E-2"/>
-          <c:w val="0.91978071330955136"/>
+          <c:w val="0.91978071330955158"/>
           <c:h val="0.89627228525119951"/>
         </c:manualLayout>
       </c:layout>
@@ -654,9 +660,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Progress!$A$48:$A$58</c:f>
+              <c:f>Progress!$A$48:$A$59</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>03-10-17</c:v>
                 </c:pt>
@@ -689,16 +695,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>06-03-17</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>06-09-17</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$B$48:$B$58</c:f>
+              <c:f>Progress!$B$48:$B$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -731,6 +740,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -763,9 +775,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Progress!$A$48:$A$58</c:f>
+              <c:f>Progress!$A$48:$A$59</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>03-10-17</c:v>
                 </c:pt>
@@ -798,16 +810,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>06-03-17</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>06-09-17</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$C$48:$C$58</c:f>
+              <c:f>Progress!$C$48:$C$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -840,6 +855,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -872,9 +890,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Progress!$A$48:$A$58</c:f>
+              <c:f>Progress!$A$48:$A$59</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>03-10-17</c:v>
                 </c:pt>
@@ -907,16 +925,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>06-03-17</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>06-09-17</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$D$48:$D$58</c:f>
+              <c:f>Progress!$D$48:$D$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -948,6 +969,9 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -981,9 +1005,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Progress!$A$47:$A$58</c:f>
+              <c:f>Progress!$A$47:$A$59</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>Date</c:v>
                 </c:pt>
@@ -1019,16 +1043,19 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>06-03-17</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>06-09-17</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$E$48:$E$58</c:f>
+              <c:f>Progress!$E$48:$E$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1060,17 +1087,20 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="154328448"/>
-        <c:axId val="153949312"/>
+        <c:axId val="151182720"/>
+        <c:axId val="150934656"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="154328448"/>
+        <c:axId val="151182720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1103,7 +1133,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153949312"/>
+        <c:crossAx val="150934656"/>
         <c:crosses val="autoZero"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
@@ -1113,7 +1143,7 @@
         <c:minorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="153949312"/>
+        <c:axId val="150934656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1155,7 +1185,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="154328448"/>
+        <c:crossAx val="151182720"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1178,7 +1208,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="6.2637362637362637E-2"/>
-          <c:y val="0.37277147487844547"/>
+          <c:y val="0.37277147487844553"/>
           <c:w val="0.12857154394162268"/>
           <c:h val="0.11669367909238262"/>
         </c:manualLayout>
@@ -1245,7 +1275,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000001332" r="0.75000000000001332" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000001343" r="0.75000000000001343" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="1200"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1299,7 +1329,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.4510450248127519E-2"/>
+          <c:x val="4.4510450248127532E-2"/>
           <c:y val="0.10032394165889739"/>
           <c:w val="0.79228601441663349"/>
           <c:h val="0.79935527708863363"/>
@@ -1334,9 +1364,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Progress!$A$48:$A$58</c:f>
+              <c:f>Progress!$A$48:$A$59</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>03-10-17</c:v>
                 </c:pt>
@@ -1369,16 +1399,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>06-03-17</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>06-09-17</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$G$48:$G$58</c:f>
+              <c:f>Progress!$G$48:$G$59</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1410,17 +1443,20 @@
                   <c:v>0.46153846153846156</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.49367088607594939</c:v>
+                  <c:v>0.46987951807228917</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.47058823529411764</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="153985408"/>
-        <c:axId val="153986944"/>
+        <c:axId val="150974848"/>
+        <c:axId val="150976384"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="153985408"/>
+        <c:axId val="150974848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1428,14 +1464,14 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd-mm-yy" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="153986944"/>
+        <c:crossAx val="150976384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153986944"/>
+        <c:axId val="150976384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1478,7 +1514,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153985408"/>
+        <c:crossAx val="150974848"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1527,7 +1563,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000001332" r="0.75000000000001332" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000001343" r="0.75000000000001343" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1578,9 +1614,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Progress!$A$48:$A$58</c:f>
+              <c:f>Progress!$A$48:$A$59</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>03-10-17</c:v>
                 </c:pt>
@@ -1613,16 +1649,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>06-03-17</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>06-09-17</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$C$48:$C$58</c:f>
+              <c:f>Progress!$C$48:$C$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1655,6 +1694,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1687,9 +1729,9 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Progress!$A$48:$A$58</c:f>
+              <c:f>Progress!$A$48:$A$59</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>03-10-17</c:v>
                 </c:pt>
@@ -1722,16 +1764,19 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>06-03-17</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>06-09-17</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$D$48:$D$58</c:f>
+              <c:f>Progress!$D$48:$D$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1763,22 +1808,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="154003712"/>
-        <c:axId val="154075136"/>
+        <c:axId val="150997248"/>
+        <c:axId val="150999040"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="154003712"/>
+        <c:axId val="150997248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m\/yyyy" sourceLinked="0"/>
+        <c:numFmt formatCode="m\/d;@" sourceLinked="0"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1806,7 +1854,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="154075136"/>
+        <c:crossAx val="150999040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1815,7 +1863,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154075136"/>
+        <c:axId val="150999040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1857,7 +1905,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="154003712"/>
+        <c:crossAx val="150997248"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1906,7 +1954,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000001332" r="0.75000000000001332" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000001343" r="0.75000000000001343" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1956,7 +2004,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1981,15 +2029,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>695324</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2364,10 +2412,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D123"/>
+  <dimension ref="A1:D128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2494,7 +2542,7 @@
     </row>
     <row r="18" spans="2:4" s="6" customFormat="1">
       <c r="B18" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>2</v>
@@ -2503,7 +2551,7 @@
     </row>
     <row r="19" spans="2:4" s="6" customFormat="1">
       <c r="B19" s="20" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>2</v>
@@ -2512,7 +2560,7 @@
     </row>
     <row r="20" spans="2:4" s="6" customFormat="1">
       <c r="B20" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>2</v>
@@ -2520,26 +2568,26 @@
       <c r="D20" s="4"/>
     </row>
     <row r="21" spans="2:4" s="6" customFormat="1">
-      <c r="B21" s="24" t="s">
-        <v>39</v>
+      <c r="B21" s="23" t="s">
+        <v>41</v>
       </c>
       <c r="C21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="2:4" s="6" customFormat="1">
+      <c r="B22" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>2</v>
-      </c>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="2:4" s="6" customFormat="1">
-      <c r="B22" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="D22" s="4"/>
     </row>
     <row r="23" spans="2:4" s="6" customFormat="1">
       <c r="B23" s="23" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>2</v>
@@ -2548,7 +2596,7 @@
     </row>
     <row r="24" spans="2:4" s="6" customFormat="1">
       <c r="B24" s="24" t="s">
-        <v>42</v>
+        <v>113</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>2</v>
@@ -2556,8 +2604,8 @@
       <c r="D24" s="4"/>
     </row>
     <row r="25" spans="2:4" s="6" customFormat="1">
-      <c r="B25" s="48" t="s">
-        <v>113</v>
+      <c r="B25" s="24" t="s">
+        <v>114</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>2</v>
@@ -2565,16 +2613,16 @@
       <c r="D25" s="4"/>
     </row>
     <row r="26" spans="2:4" s="6" customFormat="1">
-      <c r="B26" s="48" t="s">
-        <v>114</v>
+      <c r="B26" s="24" t="s">
+        <v>117</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D26" s="4"/>
     </row>
     <row r="27" spans="2:4" s="6" customFormat="1">
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="23" t="s">
         <v>43</v>
       </c>
       <c r="C27" s="7" t="s">
@@ -2583,7 +2631,7 @@
       <c r="D27" s="4"/>
     </row>
     <row r="28" spans="2:4" s="6" customFormat="1">
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="23" t="s">
         <v>96</v>
       </c>
       <c r="C28" s="7" t="s">
@@ -2592,7 +2640,7 @@
       <c r="D28" s="4"/>
     </row>
     <row r="29" spans="2:4" s="6" customFormat="1">
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="23" t="s">
         <v>101</v>
       </c>
       <c r="C29" s="7" t="s">
@@ -2601,7 +2649,7 @@
       <c r="D29" s="4"/>
     </row>
     <row r="30" spans="2:4" s="6" customFormat="1">
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="23" t="s">
         <v>102</v>
       </c>
       <c r="C30" s="7" t="s">
@@ -2610,7 +2658,7 @@
       <c r="D30" s="4"/>
     </row>
     <row r="31" spans="2:4" s="6" customFormat="1">
-      <c r="B31" s="23" t="s">
+      <c r="B31" s="20" t="s">
         <v>86</v>
       </c>
       <c r="C31" s="7" t="s">
@@ -2619,17 +2667,17 @@
       <c r="D31" s="4"/>
     </row>
     <row r="32" spans="2:4" s="6" customFormat="1">
-      <c r="B32" s="24" t="s">
-        <v>93</v>
+      <c r="B32" s="23" t="s">
+        <v>116</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D32" s="4"/>
     </row>
     <row r="33" spans="2:4" s="6" customFormat="1">
       <c r="B33" s="23" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>2</v>
@@ -2637,35 +2685,31 @@
       <c r="D33" s="4"/>
     </row>
     <row r="34" spans="2:4" s="6" customFormat="1">
-      <c r="B34" s="24" t="s">
+      <c r="B34" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="2:4" s="6" customFormat="1">
+      <c r="B35" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C35" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D34" s="4"/>
-    </row>
-    <row r="35" spans="2:4" s="6" customFormat="1">
-      <c r="B35" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>2</v>
-      </c>
       <c r="D35" s="4"/>
     </row>
     <row r="36" spans="2:4" s="6" customFormat="1">
-      <c r="B36" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B36" s="23"/>
+      <c r="C36" s="7"/>
       <c r="D36" s="4"/>
     </row>
     <row r="37" spans="2:4" s="6" customFormat="1">
-      <c r="B37" s="20" t="s">
-        <v>44</v>
+      <c r="B37" s="27" t="s">
+        <v>23</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>14</v>
@@ -2673,13 +2717,17 @@
       <c r="D37" s="4"/>
     </row>
     <row r="38" spans="2:4" s="6" customFormat="1">
-      <c r="B38" s="22"/>
-      <c r="C38" s="7"/>
+      <c r="B38" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D38" s="4"/>
     </row>
     <row r="39" spans="2:4" s="6" customFormat="1">
-      <c r="B39" s="27" t="s">
-        <v>46</v>
+      <c r="B39" s="20" t="s">
+        <v>103</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>2</v>
@@ -2688,25 +2736,21 @@
     </row>
     <row r="40" spans="2:4" s="6" customFormat="1">
       <c r="B40" s="20" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D40" s="4"/>
     </row>
     <row r="41" spans="2:4" s="6" customFormat="1">
-      <c r="B41" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>2</v>
-      </c>
+      <c r="B41" s="22"/>
+      <c r="C41" s="7"/>
       <c r="D41" s="4"/>
     </row>
     <row r="42" spans="2:4" s="6" customFormat="1">
-      <c r="B42" s="20" t="s">
-        <v>48</v>
+      <c r="B42" s="27" t="s">
+        <v>46</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>2</v>
@@ -2715,7 +2759,7 @@
     </row>
     <row r="43" spans="2:4" s="6" customFormat="1">
       <c r="B43" s="20" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>2</v>
@@ -2723,13 +2767,17 @@
       <c r="D43" s="4"/>
     </row>
     <row r="44" spans="2:4" s="6" customFormat="1">
-      <c r="B44" s="22"/>
-      <c r="C44" s="7"/>
+      <c r="B44" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D44" s="4"/>
     </row>
     <row r="45" spans="2:4" s="6" customFormat="1">
-      <c r="B45" s="27" t="s">
-        <v>50</v>
+      <c r="B45" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>2</v>
@@ -2738,7 +2786,7 @@
     </row>
     <row r="46" spans="2:4" s="6" customFormat="1">
       <c r="B46" s="20" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>2</v>
@@ -2746,71 +2794,67 @@
       <c r="D46" s="4"/>
     </row>
     <row r="47" spans="2:4" s="6" customFormat="1">
-      <c r="B47" s="20" t="s">
+      <c r="B47" s="22"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="4"/>
+    </row>
+    <row r="48" spans="2:4" s="6" customFormat="1">
+      <c r="B48" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" s="4"/>
+    </row>
+    <row r="49" spans="2:4" s="6" customFormat="1">
+      <c r="B49" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" s="4"/>
+    </row>
+    <row r="50" spans="2:4" s="6" customFormat="1">
+      <c r="B50" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C50" s="7" t="s">
         <v>2</v>
-      </c>
-      <c r="D47" s="4"/>
-    </row>
-    <row r="48" spans="2:4" s="6" customFormat="1">
-      <c r="B48" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D48" s="4"/>
-    </row>
-    <row r="49" spans="2:4" s="6" customFormat="1">
-      <c r="B49" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D49" s="4"/>
-    </row>
-    <row r="50" spans="2:4" s="6" customFormat="1">
-      <c r="B50" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="D50" s="4"/>
     </row>
     <row r="51" spans="2:4" s="6" customFormat="1">
       <c r="B51" s="23" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D51" s="4"/>
     </row>
     <row r="52" spans="2:4" s="6" customFormat="1">
       <c r="B52" s="23" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D52" s="4"/>
     </row>
     <row r="53" spans="2:4" s="6" customFormat="1">
       <c r="B53" s="23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D53" s="4"/>
     </row>
     <row r="54" spans="2:4" s="6" customFormat="1">
       <c r="B54" s="23" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>2</v>
@@ -2819,7 +2863,7 @@
     </row>
     <row r="55" spans="2:4" s="6" customFormat="1">
       <c r="B55" s="23" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>2</v>
@@ -2828,7 +2872,7 @@
     </row>
     <row r="56" spans="2:4" s="6" customFormat="1">
       <c r="B56" s="23" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>2</v>
@@ -2836,8 +2880,8 @@
       <c r="D56" s="4"/>
     </row>
     <row r="57" spans="2:4" s="6" customFormat="1">
-      <c r="B57" s="23" t="s">
-        <v>91</v>
+      <c r="B57" s="24" t="s">
+        <v>115</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>2</v>
@@ -2846,30 +2890,34 @@
     </row>
     <row r="58" spans="2:4" s="6" customFormat="1">
       <c r="B58" s="23" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D58" s="4"/>
     </row>
     <row r="59" spans="2:4" s="6" customFormat="1">
-      <c r="B59" s="23" t="s">
-        <v>65</v>
+      <c r="B59" s="24" t="s">
+        <v>115</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D59" s="4"/>
     </row>
     <row r="60" spans="2:4" s="6" customFormat="1">
-      <c r="B60" s="22"/>
-      <c r="C60" s="7"/>
+      <c r="B60" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D60" s="4"/>
     </row>
     <row r="61" spans="2:4" s="6" customFormat="1">
-      <c r="B61" s="27" t="s">
-        <v>66</v>
+      <c r="B61" s="23" t="s">
+        <v>90</v>
       </c>
       <c r="C61" s="7" t="s">
         <v>2</v>
@@ -2877,8 +2925,8 @@
       <c r="D61" s="4"/>
     </row>
     <row r="62" spans="2:4" s="6" customFormat="1">
-      <c r="B62" s="20" t="s">
-        <v>67</v>
+      <c r="B62" s="23" t="s">
+        <v>91</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>2</v>
@@ -2887,7 +2935,7 @@
     </row>
     <row r="63" spans="2:4" s="6" customFormat="1">
       <c r="B63" s="23" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>14</v>
@@ -2895,8 +2943,8 @@
       <c r="D63" s="4"/>
     </row>
     <row r="64" spans="2:4" s="6" customFormat="1">
-      <c r="B64" s="20" t="s">
-        <v>68</v>
+      <c r="B64" s="23" t="s">
+        <v>65</v>
       </c>
       <c r="C64" s="7" t="s">
         <v>14</v>
@@ -2909,23 +2957,35 @@
       <c r="D65" s="4"/>
     </row>
     <row r="66" spans="2:4" s="6" customFormat="1">
-      <c r="B66" s="22"/>
-      <c r="C66" s="7"/>
+      <c r="B66" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D66" s="4"/>
     </row>
     <row r="67" spans="2:4" s="6" customFormat="1">
-      <c r="B67" s="22"/>
-      <c r="C67" s="7"/>
+      <c r="B67" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D67" s="4"/>
     </row>
     <row r="68" spans="2:4" s="6" customFormat="1">
-      <c r="B68" s="22"/>
-      <c r="C68" s="7"/>
+      <c r="B68" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D68" s="4"/>
     </row>
     <row r="69" spans="2:4" s="6" customFormat="1">
-      <c r="B69" s="3" t="s">
-        <v>72</v>
+      <c r="B69" s="20" t="s">
+        <v>68</v>
       </c>
       <c r="C69" s="7" t="s">
         <v>14</v>
@@ -2938,21 +2998,13 @@
       <c r="D70" s="4"/>
     </row>
     <row r="71" spans="2:4" s="6" customFormat="1">
-      <c r="B71" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B71" s="22"/>
+      <c r="C71" s="7"/>
       <c r="D71" s="4"/>
     </row>
     <row r="72" spans="2:4" s="6" customFormat="1">
-      <c r="B72" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B72" s="22"/>
+      <c r="C72" s="7"/>
       <c r="D72" s="4"/>
     </row>
     <row r="73" spans="2:4" s="6" customFormat="1">
@@ -2961,18 +3013,22 @@
       <c r="D73" s="4"/>
     </row>
     <row r="74" spans="2:4" s="6" customFormat="1">
-      <c r="B74" s="19"/>
-      <c r="C74" s="4"/>
+      <c r="B74" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D74" s="4"/>
     </row>
     <row r="75" spans="2:4" s="6" customFormat="1">
-      <c r="B75" s="4"/>
-      <c r="C75" s="4"/>
+      <c r="B75" s="22"/>
+      <c r="C75" s="7"/>
       <c r="D75" s="4"/>
     </row>
     <row r="76" spans="2:4" s="6" customFormat="1">
-      <c r="B76" s="3" t="s">
-        <v>51</v>
+      <c r="B76" s="22" t="s">
+        <v>79</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>14</v>
@@ -2980,40 +3036,32 @@
       <c r="D76" s="4"/>
     </row>
     <row r="77" spans="2:4" s="6" customFormat="1">
-      <c r="B77" s="22"/>
-      <c r="C77" s="7"/>
+      <c r="B77" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D77" s="4"/>
     </row>
     <row r="78" spans="2:4" s="6" customFormat="1">
-      <c r="B78" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B78" s="22"/>
+      <c r="C78" s="7"/>
       <c r="D78" s="4"/>
     </row>
     <row r="79" spans="2:4" s="6" customFormat="1">
-      <c r="B79" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B79" s="19"/>
+      <c r="C79" s="4"/>
       <c r="D79" s="4"/>
     </row>
     <row r="80" spans="2:4" s="6" customFormat="1">
-      <c r="B80" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B80" s="4"/>
+      <c r="C80" s="4"/>
       <c r="D80" s="4"/>
     </row>
     <row r="81" spans="2:4" s="6" customFormat="1">
-      <c r="B81" s="20" t="s">
-        <v>75</v>
+      <c r="B81" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="C81" s="7" t="s">
         <v>14</v>
@@ -3021,17 +3069,13 @@
       <c r="D81" s="4"/>
     </row>
     <row r="82" spans="2:4" s="6" customFormat="1">
-      <c r="B82" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B82" s="22"/>
+      <c r="C82" s="7"/>
       <c r="D82" s="4"/>
     </row>
     <row r="83" spans="2:4" s="6" customFormat="1">
-      <c r="B83" s="20" t="s">
-        <v>107</v>
+      <c r="B83" s="22" t="s">
+        <v>52</v>
       </c>
       <c r="C83" s="7" t="s">
         <v>14</v>
@@ -3040,7 +3084,7 @@
     </row>
     <row r="84" spans="2:4" s="6" customFormat="1">
       <c r="B84" s="20" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="C84" s="7" t="s">
         <v>14</v>
@@ -3049,7 +3093,7 @@
     </row>
     <row r="85" spans="2:4" s="6" customFormat="1">
       <c r="B85" s="20" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="C85" s="7" t="s">
         <v>14</v>
@@ -3058,7 +3102,7 @@
     </row>
     <row r="86" spans="2:4" s="6" customFormat="1">
       <c r="B86" s="20" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="C86" s="7" t="s">
         <v>14</v>
@@ -3067,7 +3111,7 @@
     </row>
     <row r="87" spans="2:4" s="6" customFormat="1">
       <c r="B87" s="20" t="s">
-        <v>111</v>
+        <v>76</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>14</v>
@@ -3075,13 +3119,17 @@
       <c r="D87" s="4"/>
     </row>
     <row r="88" spans="2:4" s="6" customFormat="1">
-      <c r="B88" s="22"/>
-      <c r="C88" s="7"/>
+      <c r="B88" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D88" s="4"/>
     </row>
     <row r="89" spans="2:4" s="6" customFormat="1">
-      <c r="B89" s="22" t="s">
-        <v>53</v>
+      <c r="B89" s="20" t="s">
+        <v>108</v>
       </c>
       <c r="C89" s="7" t="s">
         <v>14</v>
@@ -3090,7 +3138,7 @@
     </row>
     <row r="90" spans="2:4" s="6" customFormat="1">
       <c r="B90" s="20" t="s">
-        <v>54</v>
+        <v>109</v>
       </c>
       <c r="C90" s="7" t="s">
         <v>14</v>
@@ -3099,7 +3147,7 @@
     </row>
     <row r="91" spans="2:4" s="6" customFormat="1">
       <c r="B91" s="20" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="C91" s="7" t="s">
         <v>14</v>
@@ -3107,42 +3155,54 @@
       <c r="D91" s="4"/>
     </row>
     <row r="92" spans="2:4" s="6" customFormat="1">
-      <c r="B92" s="22"/>
-      <c r="C92" s="7"/>
+      <c r="B92" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D92" s="4"/>
     </row>
     <row r="93" spans="2:4" s="6" customFormat="1">
-      <c r="B93" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="C93" s="7" t="s">
+      <c r="B93" s="22"/>
+      <c r="C93" s="7"/>
+      <c r="D93" s="4"/>
+    </row>
+    <row r="94" spans="2:4" s="6" customFormat="1">
+      <c r="B94" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C94" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D93" s="4"/>
-    </row>
-    <row r="94" spans="2:4" s="6" customFormat="1">
-      <c r="B94" s="22"/>
-      <c r="C94" s="7"/>
       <c r="D94" s="4"/>
     </row>
     <row r="95" spans="2:4" s="6" customFormat="1">
-      <c r="B95" s="22"/>
-      <c r="C95" s="7"/>
+      <c r="B95" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D95" s="4"/>
     </row>
     <row r="96" spans="2:4" s="6" customFormat="1">
-      <c r="B96" s="20"/>
-      <c r="C96" s="7"/>
+      <c r="B96" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D96" s="4"/>
     </row>
     <row r="97" spans="2:4" s="6" customFormat="1">
-      <c r="B97" s="20"/>
+      <c r="B97" s="22"/>
       <c r="C97" s="7"/>
       <c r="D97" s="4"/>
     </row>
     <row r="98" spans="2:4" s="6" customFormat="1">
-      <c r="B98" s="3" t="s">
-        <v>27</v>
+      <c r="B98" s="22" t="s">
+        <v>82</v>
       </c>
       <c r="C98" s="7" t="s">
         <v>14</v>
@@ -3150,45 +3210,37 @@
       <c r="D98" s="4"/>
     </row>
     <row r="99" spans="2:4" s="6" customFormat="1">
-      <c r="B99" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C99" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B99" s="22"/>
+      <c r="C99" s="7"/>
       <c r="D99" s="4"/>
     </row>
     <row r="100" spans="2:4" s="6" customFormat="1">
-      <c r="B100" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C100" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B100" s="22"/>
+      <c r="C100" s="7"/>
       <c r="D100" s="4"/>
     </row>
     <row r="101" spans="2:4" s="6" customFormat="1">
-      <c r="B101" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C101" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="B101" s="20"/>
+      <c r="C101" s="7"/>
       <c r="D101" s="4"/>
     </row>
     <row r="102" spans="2:4" s="6" customFormat="1">
-      <c r="B102" s="22"/>
+      <c r="B102" s="20"/>
       <c r="C102" s="7"/>
       <c r="D102" s="4"/>
     </row>
     <row r="103" spans="2:4" s="6" customFormat="1">
-      <c r="B103" s="22"/>
-      <c r="C103" s="7"/>
+      <c r="B103" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D103" s="4"/>
     </row>
     <row r="104" spans="2:4" s="6" customFormat="1">
-      <c r="B104" s="3" t="s">
-        <v>25</v>
+      <c r="B104" s="22" t="s">
+        <v>28</v>
       </c>
       <c r="C104" s="7" t="s">
         <v>14</v>
@@ -3197,7 +3249,7 @@
     </row>
     <row r="105" spans="2:4" s="6" customFormat="1">
       <c r="B105" s="22" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C105" s="7" t="s">
         <v>14</v>
@@ -3206,7 +3258,7 @@
     </row>
     <row r="106" spans="2:4" s="6" customFormat="1">
       <c r="B106" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C106" s="7" t="s">
         <v>14</v>
@@ -3214,27 +3266,27 @@
       <c r="D106" s="4"/>
     </row>
     <row r="107" spans="2:4" s="6" customFormat="1">
-      <c r="B107" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C107" s="7" t="s">
+      <c r="B107" s="22"/>
+      <c r="C107" s="7"/>
+      <c r="D107" s="4"/>
+    </row>
+    <row r="108" spans="2:4" s="6" customFormat="1">
+      <c r="B108" s="22"/>
+      <c r="C108" s="7"/>
+      <c r="D108" s="4"/>
+    </row>
+    <row r="109" spans="2:4" s="6" customFormat="1">
+      <c r="B109" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C109" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D107" s="4"/>
-    </row>
-    <row r="108" spans="2:4" s="6" customFormat="1">
-      <c r="B108" s="43"/>
-      <c r="C108" s="4"/>
-      <c r="D108" s="4"/>
-    </row>
-    <row r="109" spans="2:4" s="6" customFormat="1">
-      <c r="B109" s="21"/>
-      <c r="C109" s="4"/>
       <c r="D109" s="4"/>
     </row>
     <row r="110" spans="2:4" s="6" customFormat="1">
-      <c r="B110" s="3" t="s">
-        <v>19</v>
+      <c r="B110" s="22" t="s">
+        <v>26</v>
       </c>
       <c r="C110" s="7" t="s">
         <v>14</v>
@@ -3243,7 +3295,7 @@
     </row>
     <row r="111" spans="2:4" s="6" customFormat="1">
       <c r="B111" s="22" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C111" s="7" t="s">
         <v>14</v>
@@ -3252,7 +3304,7 @@
     </row>
     <row r="112" spans="2:4" s="6" customFormat="1">
       <c r="B112" s="22" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C112" s="7" t="s">
         <v>14</v>
@@ -3260,95 +3312,132 @@
       <c r="D112" s="4"/>
     </row>
     <row r="113" spans="1:4" s="6" customFormat="1">
-      <c r="B113" s="22"/>
+      <c r="B113" s="43"/>
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
     </row>
     <row r="114" spans="1:4" s="6" customFormat="1">
-      <c r="B114" s="19"/>
+      <c r="B114" s="21"/>
       <c r="C114" s="4"/>
       <c r="D114" s="4"/>
     </row>
     <row r="115" spans="1:4" s="6" customFormat="1">
-      <c r="B115" s="21"/>
-      <c r="C115" s="4"/>
+      <c r="B115" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C115" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D115" s="4"/>
     </row>
     <row r="116" spans="1:4" s="6" customFormat="1">
-      <c r="B116" s="21"/>
-      <c r="C116" s="4"/>
+      <c r="B116" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C116" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D116" s="4"/>
     </row>
-    <row r="117" spans="1:4">
-      <c r="A117" s="3"/>
-      <c r="B117" s="11"/>
-      <c r="C117" s="11"/>
-      <c r="D117" s="3"/>
-    </row>
-    <row r="118" spans="1:4">
-      <c r="A118" s="3"/>
-      <c r="B118" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C118" s="6">
-        <f>COUNTIF(C5:C117,"y")</f>
-        <v>39</v>
-      </c>
-      <c r="D118" s="2"/>
-    </row>
-    <row r="119" spans="1:4">
-      <c r="A119" s="3"/>
-      <c r="B119" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C119" s="6">
-        <f>COUNTIF(C5:C117,"n")</f>
-        <v>40</v>
-      </c>
-      <c r="D119" s="2"/>
-    </row>
-    <row r="120" spans="1:4">
-      <c r="A120" s="3"/>
-      <c r="B120" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C120" s="7">
-        <f>COUNTIF(C5:C117,"TBD")</f>
-        <v>0</v>
-      </c>
-      <c r="D120" s="2"/>
-    </row>
-    <row r="121" spans="1:4">
-      <c r="A121" s="3"/>
-      <c r="B121" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C121">
-        <f>SUM(C118:C120)</f>
-        <v>79</v>
-      </c>
-      <c r="D121" s="2"/>
-    </row>
-    <row r="122" spans="1:4" ht="18">
+    <row r="117" spans="1:4" s="6" customFormat="1">
+      <c r="B117" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C117" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D117" s="4"/>
+    </row>
+    <row r="118" spans="1:4" s="6" customFormat="1">
+      <c r="B118" s="22"/>
+      <c r="C118" s="4"/>
+      <c r="D118" s="4"/>
+    </row>
+    <row r="119" spans="1:4" s="6" customFormat="1">
+      <c r="B119" s="19"/>
+      <c r="C119" s="4"/>
+      <c r="D119" s="4"/>
+    </row>
+    <row r="120" spans="1:4" s="6" customFormat="1">
+      <c r="B120" s="21"/>
+      <c r="C120" s="4"/>
+      <c r="D120" s="4"/>
+    </row>
+    <row r="121" spans="1:4" s="6" customFormat="1">
+      <c r="B121" s="21"/>
+      <c r="C121" s="4"/>
+      <c r="D121" s="4"/>
+    </row>
+    <row r="122" spans="1:4">
       <c r="A122" s="3"/>
-      <c r="B122" s="10"/>
-      <c r="C122" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D122" s="41">
-        <f>C118/(C119+C118 + C120)</f>
-        <v>0.49367088607594939</v>
-      </c>
+      <c r="B122" s="11"/>
+      <c r="C122" s="11"/>
+      <c r="D122" s="3"/>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="3"/>
-      <c r="B123" s="11"/>
-      <c r="C123" s="11"/>
-      <c r="D123" s="3"/>
+      <c r="B123" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C123" s="6">
+        <f>COUNTIF(C5:C122,"y")</f>
+        <v>40</v>
+      </c>
+      <c r="D123" s="2"/>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" s="3"/>
+      <c r="B124" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C124" s="6">
+        <f>COUNTIF(C5:C122,"n")</f>
+        <v>43</v>
+      </c>
+      <c r="D124" s="2"/>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" s="3"/>
+      <c r="B125" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C125" s="7">
+        <f>COUNTIF(C5:C122,"TBD")</f>
+        <v>0</v>
+      </c>
+      <c r="D125" s="2"/>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" s="3"/>
+      <c r="B126" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C126">
+        <f>SUM(C123:C125)</f>
+        <v>83</v>
+      </c>
+      <c r="D126" s="2"/>
+    </row>
+    <row r="127" spans="1:4" ht="18">
+      <c r="A127" s="3"/>
+      <c r="B127" s="10"/>
+      <c r="C127" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D127" s="41">
+        <f>C123/(C124+C123 + C125)</f>
+        <v>0.48192771084337349</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" s="3"/>
+      <c r="B128" s="11"/>
+      <c r="C128" s="11"/>
+      <c r="D128" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="C1:C3 C6:C64871">
+  <conditionalFormatting sqref="C1:C3 C6:C64876">
     <cfRule type="cellIs" dxfId="2" priority="7" stopIfTrue="1" operator="equal">
       <formula>"y"</formula>
     </cfRule>
@@ -3370,12 +3459,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IT872"/>
+  <dimension ref="A1:IT873"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="10020" topLeftCell="A46" activePane="bottomLeft"/>
       <selection activeCell="O6" sqref="O6"/>
-      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
+      <selection pane="bottomLeft" activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -3704,7 +3793,7 @@
         <v>85</v>
       </c>
       <c r="G51" s="30">
-        <f t="shared" ref="G51:G57" si="2">B51/SUM(B51:E51)</f>
+        <f t="shared" ref="G51:G58" si="2">B51/SUM(B51:E51)</f>
         <v>0.37313432835820898</v>
       </c>
       <c r="H51" s="7"/>
@@ -3873,25 +3962,40 @@
         <v>0</v>
       </c>
       <c r="E58" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F58" s="28" t="s">
         <v>112</v>
       </c>
       <c r="G58" s="30">
-        <f t="shared" ref="G58" si="3">B58/SUM(B58:E58)</f>
-        <v>0.49367088607594939</v>
+        <f t="shared" si="2"/>
+        <v>0.46987951807228917</v>
       </c>
       <c r="H58" s="7"/>
     </row>
     <row r="59" spans="1:11">
-      <c r="A59" s="12"/>
-      <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="28"/>
-      <c r="G59" s="30"/>
+      <c r="A59" s="46">
+        <v>42984</v>
+      </c>
+      <c r="B59" s="4">
+        <v>40</v>
+      </c>
+      <c r="C59" s="4">
+        <v>43</v>
+      </c>
+      <c r="D59" s="4">
+        <v>0</v>
+      </c>
+      <c r="E59" s="4">
+        <v>2</v>
+      </c>
+      <c r="F59" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="G59" s="30">
+        <f t="shared" ref="G59" si="3">B59/SUM(B59:E59)</f>
+        <v>0.47058823529411764</v>
+      </c>
       <c r="H59" s="7"/>
     </row>
     <row r="60" spans="1:11">
@@ -3900,84 +4004,84 @@
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
-      <c r="F60" s="31"/>
+      <c r="F60" s="28"/>
       <c r="G60" s="30"/>
       <c r="H60" s="7"/>
     </row>
     <row r="61" spans="1:11">
-      <c r="A61" s="14" t="s">
+      <c r="A61" s="12"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="31"/>
+      <c r="G61" s="30"/>
+      <c r="H61" s="7"/>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B61" s="14" t="s">
+      <c r="B62" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C61" s="14" t="s">
+      <c r="C62" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D61" s="14" t="s">
+      <c r="D62" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E61" s="14" t="s">
+      <c r="E62" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F61" s="14" t="s">
+      <c r="F62" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G61" s="38">
-        <f>MIN(G58)</f>
-        <v>0.49367088607594939</v>
-      </c>
-      <c r="H61" s="7"/>
-    </row>
-    <row r="62" spans="1:11">
-      <c r="A62" s="39">
-        <f>SUM(B62:D62)</f>
-        <v>79</v>
-      </c>
-      <c r="B62" s="15">
-        <f>Features!C118</f>
-        <v>39</v>
-      </c>
-      <c r="C62" s="16">
-        <f>Features!C119</f>
+      <c r="G62" s="38">
+        <f>MIN(G59)</f>
+        <v>0.47058823529411764</v>
+      </c>
+      <c r="H62" s="7"/>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" s="39">
+        <f>SUM(B63:D63)</f>
+        <v>83</v>
+      </c>
+      <c r="B63" s="15">
+        <f>Features!C123</f>
         <v>40</v>
       </c>
-      <c r="D62" s="17">
-        <f>Features!C120</f>
+      <c r="C63" s="16">
+        <f>Features!C124</f>
+        <v>43</v>
+      </c>
+      <c r="D63" s="17">
+        <f>Features!C125</f>
         <v>0</v>
       </c>
-      <c r="E62" s="18">
-        <f>MIN(E58)</f>
-        <v>0</v>
-      </c>
-      <c r="F62" s="7"/>
-      <c r="G62" s="30"/>
-      <c r="H62" s="7"/>
-    </row>
-    <row r="63" spans="1:11">
-      <c r="A63" s="4"/>
-      <c r="B63" s="19"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7"/>
+      <c r="E63" s="18">
+        <f>MIN(E59)</f>
+        <v>2</v>
+      </c>
       <c r="F63" s="7"/>
       <c r="G63" s="30"/>
       <c r="H63" s="7"/>
-      <c r="J63" s="36"/>
     </row>
     <row r="64" spans="1:11">
       <c r="A64" s="4"/>
-      <c r="B64" s="4"/>
+      <c r="B64" s="19"/>
       <c r="C64" s="4"/>
       <c r="D64" s="7"/>
       <c r="E64" s="7"/>
       <c r="F64" s="7"/>
       <c r="G64" s="30"/>
       <c r="H64" s="7"/>
+      <c r="J64" s="36"/>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" s="4"/>
-      <c r="B65" s="19"/>
+      <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="7"/>
       <c r="E65" s="7"/>
@@ -3987,7 +4091,7 @@
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="4"/>
-      <c r="B66" s="4"/>
+      <c r="B66" s="19"/>
       <c r="C66" s="4"/>
       <c r="D66" s="7"/>
       <c r="E66" s="7"/>
@@ -4007,7 +4111,7 @@
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="4"/>
-      <c r="B68" s="19"/>
+      <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="7"/>
       <c r="E68" s="7"/>
@@ -4027,7 +4131,7 @@
     </row>
     <row r="70" spans="1:8">
       <c r="A70" s="4"/>
-      <c r="B70" s="4"/>
+      <c r="B70" s="19"/>
       <c r="C70" s="4"/>
       <c r="D70" s="7"/>
       <c r="E70" s="7"/>
@@ -4047,7 +4151,7 @@
     </row>
     <row r="72" spans="1:8">
       <c r="A72" s="4"/>
-      <c r="B72" s="7"/>
+      <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="7"/>
       <c r="E72" s="7"/>
@@ -4057,7 +4161,7 @@
     </row>
     <row r="73" spans="1:8">
       <c r="A73" s="4"/>
-      <c r="B73" s="20"/>
+      <c r="B73" s="7"/>
       <c r="C73" s="4"/>
       <c r="D73" s="7"/>
       <c r="E73" s="7"/>
@@ -4076,7 +4180,7 @@
       <c r="H74" s="7"/>
     </row>
     <row r="75" spans="1:8">
-      <c r="A75" s="7"/>
+      <c r="A75" s="4"/>
       <c r="B75" s="20"/>
       <c r="C75" s="4"/>
       <c r="D75" s="7"/>
@@ -4087,7 +4191,7 @@
     </row>
     <row r="76" spans="1:8">
       <c r="A76" s="7"/>
-      <c r="B76" s="7"/>
+      <c r="B76" s="20"/>
       <c r="C76" s="4"/>
       <c r="D76" s="7"/>
       <c r="E76" s="7"/>
@@ -4218,7 +4322,7 @@
     <row r="89" spans="1:8">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
-      <c r="C89" s="7"/>
+      <c r="C89" s="4"/>
       <c r="D89" s="7"/>
       <c r="E89" s="7"/>
       <c r="F89" s="7"/>
@@ -4227,7 +4331,7 @@
     </row>
     <row r="90" spans="1:8">
       <c r="A90" s="7"/>
-      <c r="B90" s="6"/>
+      <c r="B90" s="7"/>
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
       <c r="E90" s="7"/>
@@ -4235,15 +4339,15 @@
       <c r="G90" s="30"/>
       <c r="H90" s="7"/>
     </row>
-    <row r="91" spans="1:8" s="2" customFormat="1">
-      <c r="A91" s="4"/>
-      <c r="B91" s="4"/>
-      <c r="C91" s="4"/>
-      <c r="D91" s="4"/>
-      <c r="E91" s="4"/>
-      <c r="F91" s="4"/>
-      <c r="G91" s="34"/>
-      <c r="H91" s="4"/>
+    <row r="91" spans="1:8">
+      <c r="A91" s="7"/>
+      <c r="B91" s="6"/>
+      <c r="C91" s="7"/>
+      <c r="D91" s="7"/>
+      <c r="E91" s="7"/>
+      <c r="F91" s="7"/>
+      <c r="G91" s="30"/>
+      <c r="H91" s="7"/>
     </row>
     <row r="92" spans="1:8" s="2" customFormat="1">
       <c r="A92" s="4"/>
@@ -4417,7 +4521,7 @@
     </row>
     <row r="109" spans="1:8" s="2" customFormat="1">
       <c r="A109" s="4"/>
-      <c r="B109" s="6"/>
+      <c r="B109" s="4"/>
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
       <c r="E109" s="4"/>
@@ -4427,7 +4531,7 @@
     </row>
     <row r="110" spans="1:8" s="2" customFormat="1">
       <c r="A110" s="4"/>
-      <c r="B110" s="4"/>
+      <c r="B110" s="6"/>
       <c r="C110" s="4"/>
       <c r="D110" s="4"/>
       <c r="E110" s="4"/>
@@ -4457,7 +4561,7 @@
     </row>
     <row r="113" spans="1:8" s="2" customFormat="1">
       <c r="A113" s="4"/>
-      <c r="B113" s="19"/>
+      <c r="B113" s="4"/>
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
       <c r="E113" s="4"/>
@@ -4497,7 +4601,7 @@
     </row>
     <row r="117" spans="1:8" s="2" customFormat="1">
       <c r="A117" s="4"/>
-      <c r="B117" s="21"/>
+      <c r="B117" s="19"/>
       <c r="C117" s="4"/>
       <c r="D117" s="4"/>
       <c r="E117" s="4"/>
@@ -4507,7 +4611,7 @@
     </row>
     <row r="118" spans="1:8" s="2" customFormat="1">
       <c r="A118" s="4"/>
-      <c r="B118" s="4"/>
+      <c r="B118" s="21"/>
       <c r="C118" s="4"/>
       <c r="D118" s="4"/>
       <c r="E118" s="4"/>
@@ -4517,7 +4621,7 @@
     </row>
     <row r="119" spans="1:8" s="2" customFormat="1">
       <c r="A119" s="4"/>
-      <c r="B119" s="6"/>
+      <c r="B119" s="4"/>
       <c r="C119" s="4"/>
       <c r="D119" s="4"/>
       <c r="E119" s="4"/>
@@ -4527,7 +4631,7 @@
     </row>
     <row r="120" spans="1:8" s="2" customFormat="1">
       <c r="A120" s="4"/>
-      <c r="B120" s="4"/>
+      <c r="B120" s="6"/>
       <c r="C120" s="4"/>
       <c r="D120" s="4"/>
       <c r="E120" s="4"/>
@@ -4537,7 +4641,7 @@
     </row>
     <row r="121" spans="1:8" s="2" customFormat="1">
       <c r="A121" s="4"/>
-      <c r="B121" s="19"/>
+      <c r="B121" s="4"/>
       <c r="C121" s="4"/>
       <c r="D121" s="4"/>
       <c r="E121" s="4"/>
@@ -4557,7 +4661,7 @@
     </row>
     <row r="123" spans="1:8" s="2" customFormat="1">
       <c r="A123" s="4"/>
-      <c r="B123" s="4"/>
+      <c r="B123" s="19"/>
       <c r="C123" s="4"/>
       <c r="D123" s="4"/>
       <c r="E123" s="4"/>
@@ -4617,7 +4721,7 @@
     </row>
     <row r="129" spans="1:8" s="2" customFormat="1">
       <c r="A129" s="4"/>
-      <c r="B129" s="19"/>
+      <c r="B129" s="4"/>
       <c r="C129" s="4"/>
       <c r="D129" s="4"/>
       <c r="E129" s="4"/>
@@ -4717,7 +4821,7 @@
     </row>
     <row r="139" spans="1:8" s="2" customFormat="1">
       <c r="A139" s="4"/>
-      <c r="B139" s="4"/>
+      <c r="B139" s="19"/>
       <c r="C139" s="4"/>
       <c r="D139" s="4"/>
       <c r="E139" s="4"/>
@@ -4767,7 +4871,7 @@
     </row>
     <row r="144" spans="1:8" s="2" customFormat="1">
       <c r="A144" s="4"/>
-      <c r="B144" s="19"/>
+      <c r="B144" s="4"/>
       <c r="C144" s="4"/>
       <c r="D144" s="4"/>
       <c r="E144" s="4"/>
@@ -4787,7 +4891,7 @@
     </row>
     <row r="146" spans="1:254" s="2" customFormat="1">
       <c r="A146" s="4"/>
-      <c r="B146" s="4"/>
+      <c r="B146" s="19"/>
       <c r="C146" s="4"/>
       <c r="D146" s="4"/>
       <c r="E146" s="4"/>
@@ -4826,284 +4930,284 @@
       <c r="H149" s="4"/>
     </row>
     <row r="150" spans="1:254" s="2" customFormat="1">
-      <c r="A150" s="21"/>
-      <c r="B150" s="21"/>
-      <c r="C150" s="21"/>
-      <c r="D150" s="21"/>
-      <c r="E150" s="21"/>
-      <c r="F150" s="21"/>
-      <c r="G150" s="35"/>
-      <c r="H150" s="21"/>
-      <c r="I150" s="5"/>
-      <c r="J150" s="5"/>
-      <c r="K150" s="5"/>
-      <c r="L150" s="5"/>
-      <c r="M150" s="5"/>
-      <c r="N150" s="5"/>
-      <c r="O150" s="5"/>
-      <c r="P150" s="5"/>
-      <c r="Q150" s="5"/>
-      <c r="R150" s="5"/>
-      <c r="S150" s="5"/>
-      <c r="T150" s="5"/>
-      <c r="U150" s="5"/>
-      <c r="V150" s="5"/>
-      <c r="W150" s="5"/>
-      <c r="X150" s="5"/>
-      <c r="Y150" s="5"/>
-      <c r="Z150" s="5"/>
-      <c r="AA150" s="5"/>
-      <c r="AB150" s="5"/>
-      <c r="AC150" s="5"/>
-      <c r="AD150" s="5"/>
-      <c r="AE150" s="5"/>
-      <c r="AF150" s="5"/>
-      <c r="AG150" s="5"/>
-      <c r="AH150" s="5"/>
-      <c r="AI150" s="5"/>
-      <c r="AJ150" s="5"/>
-      <c r="AK150" s="5"/>
-      <c r="AL150" s="5"/>
-      <c r="AM150" s="5"/>
-      <c r="AN150" s="5"/>
-      <c r="AO150" s="5"/>
-      <c r="AP150" s="5"/>
-      <c r="AQ150" s="5"/>
-      <c r="AR150" s="5"/>
-      <c r="AS150" s="5"/>
-      <c r="AT150" s="5"/>
-      <c r="AU150" s="5"/>
-      <c r="AV150" s="5"/>
-      <c r="AW150" s="5"/>
-      <c r="AX150" s="5"/>
-      <c r="AY150" s="5"/>
-      <c r="AZ150" s="5"/>
-      <c r="BA150" s="5"/>
-      <c r="BB150" s="5"/>
-      <c r="BC150" s="5"/>
-      <c r="BD150" s="5"/>
-      <c r="BE150" s="5"/>
-      <c r="BF150" s="5"/>
-      <c r="BG150" s="5"/>
-      <c r="BH150" s="5"/>
-      <c r="BI150" s="5"/>
-      <c r="BJ150" s="5"/>
-      <c r="BK150" s="5"/>
-      <c r="BL150" s="5"/>
-      <c r="BM150" s="5"/>
-      <c r="BN150" s="5"/>
-      <c r="BO150" s="5"/>
-      <c r="BP150" s="5"/>
-      <c r="BQ150" s="5"/>
-      <c r="BR150" s="5"/>
-      <c r="BS150" s="5"/>
-      <c r="BT150" s="5"/>
-      <c r="BU150" s="5"/>
-      <c r="BV150" s="5"/>
-      <c r="BW150" s="5"/>
-      <c r="BX150" s="5"/>
-      <c r="BY150" s="5"/>
-      <c r="BZ150" s="5"/>
-      <c r="CA150" s="5"/>
-      <c r="CB150" s="5"/>
-      <c r="CC150" s="5"/>
-      <c r="CD150" s="5"/>
-      <c r="CE150" s="5"/>
-      <c r="CF150" s="5"/>
-      <c r="CG150" s="5"/>
-      <c r="CH150" s="5"/>
-      <c r="CI150" s="5"/>
-      <c r="CJ150" s="5"/>
-      <c r="CK150" s="5"/>
-      <c r="CL150" s="5"/>
-      <c r="CM150" s="5"/>
-      <c r="CN150" s="5"/>
-      <c r="CO150" s="5"/>
-      <c r="CP150" s="5"/>
-      <c r="CQ150" s="5"/>
-      <c r="CR150" s="5"/>
-      <c r="CS150" s="5"/>
-      <c r="CT150" s="5"/>
-      <c r="CU150" s="5"/>
-      <c r="CV150" s="5"/>
-      <c r="CW150" s="5"/>
-      <c r="CX150" s="5"/>
-      <c r="CY150" s="5"/>
-      <c r="CZ150" s="5"/>
-      <c r="DA150" s="5"/>
-      <c r="DB150" s="5"/>
-      <c r="DC150" s="5"/>
-      <c r="DD150" s="5"/>
-      <c r="DE150" s="5"/>
-      <c r="DF150" s="5"/>
-      <c r="DG150" s="5"/>
-      <c r="DH150" s="5"/>
-      <c r="DI150" s="5"/>
-      <c r="DJ150" s="5"/>
-      <c r="DK150" s="5"/>
-      <c r="DL150" s="5"/>
-      <c r="DM150" s="5"/>
-      <c r="DN150" s="5"/>
-      <c r="DO150" s="5"/>
-      <c r="DP150" s="5"/>
-      <c r="DQ150" s="5"/>
-      <c r="DR150" s="5"/>
-      <c r="DS150" s="5"/>
-      <c r="DT150" s="5"/>
-      <c r="DU150" s="5"/>
-      <c r="DV150" s="5"/>
-      <c r="DW150" s="5"/>
-      <c r="DX150" s="5"/>
-      <c r="DY150" s="5"/>
-      <c r="DZ150" s="5"/>
-      <c r="EA150" s="5"/>
-      <c r="EB150" s="5"/>
-      <c r="EC150" s="5"/>
-      <c r="ED150" s="5"/>
-      <c r="EE150" s="5"/>
-      <c r="EF150" s="5"/>
-      <c r="EG150" s="5"/>
-      <c r="EH150" s="5"/>
-      <c r="EI150" s="5"/>
-      <c r="EJ150" s="5"/>
-      <c r="EK150" s="5"/>
-      <c r="EL150" s="5"/>
-      <c r="EM150" s="5"/>
-      <c r="EN150" s="5"/>
-      <c r="EO150" s="5"/>
-      <c r="EP150" s="5"/>
-      <c r="EQ150" s="5"/>
-      <c r="ER150" s="5"/>
-      <c r="ES150" s="5"/>
-      <c r="ET150" s="5"/>
-      <c r="EU150" s="5"/>
-      <c r="EV150" s="5"/>
-      <c r="EW150" s="5"/>
-      <c r="EX150" s="5"/>
-      <c r="EY150" s="5"/>
-      <c r="EZ150" s="5"/>
-      <c r="FA150" s="5"/>
-      <c r="FB150" s="5"/>
-      <c r="FC150" s="5"/>
-      <c r="FD150" s="5"/>
-      <c r="FE150" s="5"/>
-      <c r="FF150" s="5"/>
-      <c r="FG150" s="5"/>
-      <c r="FH150" s="5"/>
-      <c r="FI150" s="5"/>
-      <c r="FJ150" s="5"/>
-      <c r="FK150" s="5"/>
-      <c r="FL150" s="5"/>
-      <c r="FM150" s="5"/>
-      <c r="FN150" s="5"/>
-      <c r="FO150" s="5"/>
-      <c r="FP150" s="5"/>
-      <c r="FQ150" s="5"/>
-      <c r="FR150" s="5"/>
-      <c r="FS150" s="5"/>
-      <c r="FT150" s="5"/>
-      <c r="FU150" s="5"/>
-      <c r="FV150" s="5"/>
-      <c r="FW150" s="5"/>
-      <c r="FX150" s="5"/>
-      <c r="FY150" s="5"/>
-      <c r="FZ150" s="5"/>
-      <c r="GA150" s="5"/>
-      <c r="GB150" s="5"/>
-      <c r="GC150" s="5"/>
-      <c r="GD150" s="5"/>
-      <c r="GE150" s="5"/>
-      <c r="GF150" s="5"/>
-      <c r="GG150" s="5"/>
-      <c r="GH150" s="5"/>
-      <c r="GI150" s="5"/>
-      <c r="GJ150" s="5"/>
-      <c r="GK150" s="5"/>
-      <c r="GL150" s="5"/>
-      <c r="GM150" s="5"/>
-      <c r="GN150" s="5"/>
-      <c r="GO150" s="5"/>
-      <c r="GP150" s="5"/>
-      <c r="GQ150" s="5"/>
-      <c r="GR150" s="5"/>
-      <c r="GS150" s="5"/>
-      <c r="GT150" s="5"/>
-      <c r="GU150" s="5"/>
-      <c r="GV150" s="5"/>
-      <c r="GW150" s="5"/>
-      <c r="GX150" s="5"/>
-      <c r="GY150" s="5"/>
-      <c r="GZ150" s="5"/>
-      <c r="HA150" s="5"/>
-      <c r="HB150" s="5"/>
-      <c r="HC150" s="5"/>
-      <c r="HD150" s="5"/>
-      <c r="HE150" s="5"/>
-      <c r="HF150" s="5"/>
-      <c r="HG150" s="5"/>
-      <c r="HH150" s="5"/>
-      <c r="HI150" s="5"/>
-      <c r="HJ150" s="5"/>
-      <c r="HK150" s="5"/>
-      <c r="HL150" s="5"/>
-      <c r="HM150" s="5"/>
-      <c r="HN150" s="5"/>
-      <c r="HO150" s="5"/>
-      <c r="HP150" s="5"/>
-      <c r="HQ150" s="5"/>
-      <c r="HR150" s="5"/>
-      <c r="HS150" s="5"/>
-      <c r="HT150" s="5"/>
-      <c r="HU150" s="5"/>
-      <c r="HV150" s="5"/>
-      <c r="HW150" s="5"/>
-      <c r="HX150" s="5"/>
-      <c r="HY150" s="5"/>
-      <c r="HZ150" s="5"/>
-      <c r="IA150" s="5"/>
-      <c r="IB150" s="5"/>
-      <c r="IC150" s="5"/>
-      <c r="ID150" s="5"/>
-      <c r="IE150" s="5"/>
-      <c r="IF150" s="5"/>
-      <c r="IG150" s="5"/>
-      <c r="IH150" s="5"/>
-      <c r="II150" s="5"/>
-      <c r="IJ150" s="5"/>
-      <c r="IK150" s="5"/>
-      <c r="IL150" s="5"/>
-      <c r="IM150" s="5"/>
-      <c r="IN150" s="5"/>
-      <c r="IO150" s="5"/>
-      <c r="IP150" s="5"/>
-      <c r="IQ150" s="5"/>
-      <c r="IR150" s="5"/>
-      <c r="IS150" s="5"/>
-      <c r="IT150" s="5"/>
+      <c r="A150" s="4"/>
+      <c r="B150" s="4"/>
+      <c r="C150" s="4"/>
+      <c r="D150" s="4"/>
+      <c r="E150" s="4"/>
+      <c r="F150" s="4"/>
+      <c r="G150" s="34"/>
+      <c r="H150" s="4"/>
     </row>
     <row r="151" spans="1:254" s="2" customFormat="1">
-      <c r="A151" s="4"/>
-      <c r="B151" s="4"/>
-      <c r="C151" s="4"/>
-      <c r="D151" s="4"/>
-      <c r="E151" s="4"/>
-      <c r="F151" s="4"/>
-      <c r="G151" s="34"/>
-      <c r="H151" s="4"/>
-    </row>
-    <row r="152" spans="1:254">
-      <c r="A152" s="7"/>
-      <c r="B152" s="6"/>
-      <c r="C152" s="7"/>
-      <c r="D152" s="7"/>
-      <c r="E152" s="7"/>
-      <c r="F152" s="7"/>
-      <c r="G152" s="30"/>
-      <c r="H152" s="7"/>
+      <c r="A151" s="21"/>
+      <c r="B151" s="21"/>
+      <c r="C151" s="21"/>
+      <c r="D151" s="21"/>
+      <c r="E151" s="21"/>
+      <c r="F151" s="21"/>
+      <c r="G151" s="35"/>
+      <c r="H151" s="21"/>
+      <c r="I151" s="5"/>
+      <c r="J151" s="5"/>
+      <c r="K151" s="5"/>
+      <c r="L151" s="5"/>
+      <c r="M151" s="5"/>
+      <c r="N151" s="5"/>
+      <c r="O151" s="5"/>
+      <c r="P151" s="5"/>
+      <c r="Q151" s="5"/>
+      <c r="R151" s="5"/>
+      <c r="S151" s="5"/>
+      <c r="T151" s="5"/>
+      <c r="U151" s="5"/>
+      <c r="V151" s="5"/>
+      <c r="W151" s="5"/>
+      <c r="X151" s="5"/>
+      <c r="Y151" s="5"/>
+      <c r="Z151" s="5"/>
+      <c r="AA151" s="5"/>
+      <c r="AB151" s="5"/>
+      <c r="AC151" s="5"/>
+      <c r="AD151" s="5"/>
+      <c r="AE151" s="5"/>
+      <c r="AF151" s="5"/>
+      <c r="AG151" s="5"/>
+      <c r="AH151" s="5"/>
+      <c r="AI151" s="5"/>
+      <c r="AJ151" s="5"/>
+      <c r="AK151" s="5"/>
+      <c r="AL151" s="5"/>
+      <c r="AM151" s="5"/>
+      <c r="AN151" s="5"/>
+      <c r="AO151" s="5"/>
+      <c r="AP151" s="5"/>
+      <c r="AQ151" s="5"/>
+      <c r="AR151" s="5"/>
+      <c r="AS151" s="5"/>
+      <c r="AT151" s="5"/>
+      <c r="AU151" s="5"/>
+      <c r="AV151" s="5"/>
+      <c r="AW151" s="5"/>
+      <c r="AX151" s="5"/>
+      <c r="AY151" s="5"/>
+      <c r="AZ151" s="5"/>
+      <c r="BA151" s="5"/>
+      <c r="BB151" s="5"/>
+      <c r="BC151" s="5"/>
+      <c r="BD151" s="5"/>
+      <c r="BE151" s="5"/>
+      <c r="BF151" s="5"/>
+      <c r="BG151" s="5"/>
+      <c r="BH151" s="5"/>
+      <c r="BI151" s="5"/>
+      <c r="BJ151" s="5"/>
+      <c r="BK151" s="5"/>
+      <c r="BL151" s="5"/>
+      <c r="BM151" s="5"/>
+      <c r="BN151" s="5"/>
+      <c r="BO151" s="5"/>
+      <c r="BP151" s="5"/>
+      <c r="BQ151" s="5"/>
+      <c r="BR151" s="5"/>
+      <c r="BS151" s="5"/>
+      <c r="BT151" s="5"/>
+      <c r="BU151" s="5"/>
+      <c r="BV151" s="5"/>
+      <c r="BW151" s="5"/>
+      <c r="BX151" s="5"/>
+      <c r="BY151" s="5"/>
+      <c r="BZ151" s="5"/>
+      <c r="CA151" s="5"/>
+      <c r="CB151" s="5"/>
+      <c r="CC151" s="5"/>
+      <c r="CD151" s="5"/>
+      <c r="CE151" s="5"/>
+      <c r="CF151" s="5"/>
+      <c r="CG151" s="5"/>
+      <c r="CH151" s="5"/>
+      <c r="CI151" s="5"/>
+      <c r="CJ151" s="5"/>
+      <c r="CK151" s="5"/>
+      <c r="CL151" s="5"/>
+      <c r="CM151" s="5"/>
+      <c r="CN151" s="5"/>
+      <c r="CO151" s="5"/>
+      <c r="CP151" s="5"/>
+      <c r="CQ151" s="5"/>
+      <c r="CR151" s="5"/>
+      <c r="CS151" s="5"/>
+      <c r="CT151" s="5"/>
+      <c r="CU151" s="5"/>
+      <c r="CV151" s="5"/>
+      <c r="CW151" s="5"/>
+      <c r="CX151" s="5"/>
+      <c r="CY151" s="5"/>
+      <c r="CZ151" s="5"/>
+      <c r="DA151" s="5"/>
+      <c r="DB151" s="5"/>
+      <c r="DC151" s="5"/>
+      <c r="DD151" s="5"/>
+      <c r="DE151" s="5"/>
+      <c r="DF151" s="5"/>
+      <c r="DG151" s="5"/>
+      <c r="DH151" s="5"/>
+      <c r="DI151" s="5"/>
+      <c r="DJ151" s="5"/>
+      <c r="DK151" s="5"/>
+      <c r="DL151" s="5"/>
+      <c r="DM151" s="5"/>
+      <c r="DN151" s="5"/>
+      <c r="DO151" s="5"/>
+      <c r="DP151" s="5"/>
+      <c r="DQ151" s="5"/>
+      <c r="DR151" s="5"/>
+      <c r="DS151" s="5"/>
+      <c r="DT151" s="5"/>
+      <c r="DU151" s="5"/>
+      <c r="DV151" s="5"/>
+      <c r="DW151" s="5"/>
+      <c r="DX151" s="5"/>
+      <c r="DY151" s="5"/>
+      <c r="DZ151" s="5"/>
+      <c r="EA151" s="5"/>
+      <c r="EB151" s="5"/>
+      <c r="EC151" s="5"/>
+      <c r="ED151" s="5"/>
+      <c r="EE151" s="5"/>
+      <c r="EF151" s="5"/>
+      <c r="EG151" s="5"/>
+      <c r="EH151" s="5"/>
+      <c r="EI151" s="5"/>
+      <c r="EJ151" s="5"/>
+      <c r="EK151" s="5"/>
+      <c r="EL151" s="5"/>
+      <c r="EM151" s="5"/>
+      <c r="EN151" s="5"/>
+      <c r="EO151" s="5"/>
+      <c r="EP151" s="5"/>
+      <c r="EQ151" s="5"/>
+      <c r="ER151" s="5"/>
+      <c r="ES151" s="5"/>
+      <c r="ET151" s="5"/>
+      <c r="EU151" s="5"/>
+      <c r="EV151" s="5"/>
+      <c r="EW151" s="5"/>
+      <c r="EX151" s="5"/>
+      <c r="EY151" s="5"/>
+      <c r="EZ151" s="5"/>
+      <c r="FA151" s="5"/>
+      <c r="FB151" s="5"/>
+      <c r="FC151" s="5"/>
+      <c r="FD151" s="5"/>
+      <c r="FE151" s="5"/>
+      <c r="FF151" s="5"/>
+      <c r="FG151" s="5"/>
+      <c r="FH151" s="5"/>
+      <c r="FI151" s="5"/>
+      <c r="FJ151" s="5"/>
+      <c r="FK151" s="5"/>
+      <c r="FL151" s="5"/>
+      <c r="FM151" s="5"/>
+      <c r="FN151" s="5"/>
+      <c r="FO151" s="5"/>
+      <c r="FP151" s="5"/>
+      <c r="FQ151" s="5"/>
+      <c r="FR151" s="5"/>
+      <c r="FS151" s="5"/>
+      <c r="FT151" s="5"/>
+      <c r="FU151" s="5"/>
+      <c r="FV151" s="5"/>
+      <c r="FW151" s="5"/>
+      <c r="FX151" s="5"/>
+      <c r="FY151" s="5"/>
+      <c r="FZ151" s="5"/>
+      <c r="GA151" s="5"/>
+      <c r="GB151" s="5"/>
+      <c r="GC151" s="5"/>
+      <c r="GD151" s="5"/>
+      <c r="GE151" s="5"/>
+      <c r="GF151" s="5"/>
+      <c r="GG151" s="5"/>
+      <c r="GH151" s="5"/>
+      <c r="GI151" s="5"/>
+      <c r="GJ151" s="5"/>
+      <c r="GK151" s="5"/>
+      <c r="GL151" s="5"/>
+      <c r="GM151" s="5"/>
+      <c r="GN151" s="5"/>
+      <c r="GO151" s="5"/>
+      <c r="GP151" s="5"/>
+      <c r="GQ151" s="5"/>
+      <c r="GR151" s="5"/>
+      <c r="GS151" s="5"/>
+      <c r="GT151" s="5"/>
+      <c r="GU151" s="5"/>
+      <c r="GV151" s="5"/>
+      <c r="GW151" s="5"/>
+      <c r="GX151" s="5"/>
+      <c r="GY151" s="5"/>
+      <c r="GZ151" s="5"/>
+      <c r="HA151" s="5"/>
+      <c r="HB151" s="5"/>
+      <c r="HC151" s="5"/>
+      <c r="HD151" s="5"/>
+      <c r="HE151" s="5"/>
+      <c r="HF151" s="5"/>
+      <c r="HG151" s="5"/>
+      <c r="HH151" s="5"/>
+      <c r="HI151" s="5"/>
+      <c r="HJ151" s="5"/>
+      <c r="HK151" s="5"/>
+      <c r="HL151" s="5"/>
+      <c r="HM151" s="5"/>
+      <c r="HN151" s="5"/>
+      <c r="HO151" s="5"/>
+      <c r="HP151" s="5"/>
+      <c r="HQ151" s="5"/>
+      <c r="HR151" s="5"/>
+      <c r="HS151" s="5"/>
+      <c r="HT151" s="5"/>
+      <c r="HU151" s="5"/>
+      <c r="HV151" s="5"/>
+      <c r="HW151" s="5"/>
+      <c r="HX151" s="5"/>
+      <c r="HY151" s="5"/>
+      <c r="HZ151" s="5"/>
+      <c r="IA151" s="5"/>
+      <c r="IB151" s="5"/>
+      <c r="IC151" s="5"/>
+      <c r="ID151" s="5"/>
+      <c r="IE151" s="5"/>
+      <c r="IF151" s="5"/>
+      <c r="IG151" s="5"/>
+      <c r="IH151" s="5"/>
+      <c r="II151" s="5"/>
+      <c r="IJ151" s="5"/>
+      <c r="IK151" s="5"/>
+      <c r="IL151" s="5"/>
+      <c r="IM151" s="5"/>
+      <c r="IN151" s="5"/>
+      <c r="IO151" s="5"/>
+      <c r="IP151" s="5"/>
+      <c r="IQ151" s="5"/>
+      <c r="IR151" s="5"/>
+      <c r="IS151" s="5"/>
+      <c r="IT151" s="5"/>
+    </row>
+    <row r="152" spans="1:254" s="2" customFormat="1">
+      <c r="A152" s="4"/>
+      <c r="B152" s="4"/>
+      <c r="C152" s="4"/>
+      <c r="D152" s="4"/>
+      <c r="E152" s="4"/>
+      <c r="F152" s="4"/>
+      <c r="G152" s="34"/>
+      <c r="H152" s="4"/>
     </row>
     <row r="153" spans="1:254">
       <c r="A153" s="7"/>
-      <c r="B153" s="7"/>
+      <c r="B153" s="6"/>
       <c r="C153" s="7"/>
       <c r="D153" s="7"/>
       <c r="E153" s="7"/>
@@ -5113,7 +5217,7 @@
     </row>
     <row r="154" spans="1:254">
       <c r="A154" s="7"/>
-      <c r="B154" s="20"/>
+      <c r="B154" s="7"/>
       <c r="C154" s="7"/>
       <c r="D154" s="7"/>
       <c r="E154" s="7"/>
@@ -5123,7 +5227,7 @@
     </row>
     <row r="155" spans="1:254">
       <c r="A155" s="7"/>
-      <c r="B155" s="7"/>
+      <c r="B155" s="20"/>
       <c r="C155" s="7"/>
       <c r="D155" s="7"/>
       <c r="E155" s="7"/>
@@ -5134,7 +5238,7 @@
     <row r="156" spans="1:254">
       <c r="A156" s="7"/>
       <c r="B156" s="7"/>
-      <c r="C156" s="4"/>
+      <c r="C156" s="7"/>
       <c r="D156" s="7"/>
       <c r="E156" s="7"/>
       <c r="F156" s="7"/>
@@ -5174,7 +5278,7 @@
     <row r="160" spans="1:254">
       <c r="A160" s="7"/>
       <c r="B160" s="7"/>
-      <c r="C160" s="7"/>
+      <c r="C160" s="4"/>
       <c r="D160" s="7"/>
       <c r="E160" s="7"/>
       <c r="F160" s="7"/>
@@ -5183,7 +5287,7 @@
     </row>
     <row r="161" spans="1:8">
       <c r="A161" s="7"/>
-      <c r="B161" s="22"/>
+      <c r="B161" s="7"/>
       <c r="C161" s="7"/>
       <c r="D161" s="7"/>
       <c r="E161" s="7"/>
@@ -5203,7 +5307,7 @@
     </row>
     <row r="163" spans="1:8">
       <c r="A163" s="7"/>
-      <c r="B163" s="7"/>
+      <c r="B163" s="22"/>
       <c r="C163" s="7"/>
       <c r="D163" s="7"/>
       <c r="E163" s="7"/>
@@ -5213,7 +5317,7 @@
     </row>
     <row r="164" spans="1:8">
       <c r="A164" s="7"/>
-      <c r="B164" s="20"/>
+      <c r="B164" s="7"/>
       <c r="C164" s="7"/>
       <c r="D164" s="7"/>
       <c r="E164" s="7"/>
@@ -5233,7 +5337,7 @@
     </row>
     <row r="166" spans="1:8">
       <c r="A166" s="7"/>
-      <c r="B166" s="7"/>
+      <c r="B166" s="20"/>
       <c r="C166" s="7"/>
       <c r="D166" s="7"/>
       <c r="E166" s="7"/>
@@ -5253,7 +5357,7 @@
     </row>
     <row r="168" spans="1:8">
       <c r="A168" s="7"/>
-      <c r="B168" s="20"/>
+      <c r="B168" s="7"/>
       <c r="C168" s="7"/>
       <c r="D168" s="7"/>
       <c r="E168" s="7"/>
@@ -5272,10 +5376,8 @@
       <c r="H169" s="7"/>
     </row>
     <row r="170" spans="1:8">
-      <c r="A170" s="45">
-        <v>43011</v>
-      </c>
-      <c r="B170" s="7"/>
+      <c r="A170" s="7"/>
+      <c r="B170" s="20"/>
       <c r="C170" s="7"/>
       <c r="D170" s="7"/>
       <c r="E170" s="7"/>
@@ -5284,7 +5386,9 @@
       <c r="H170" s="7"/>
     </row>
     <row r="171" spans="1:8">
-      <c r="A171" s="7"/>
+      <c r="A171" s="45">
+        <v>43011</v>
+      </c>
       <c r="B171" s="7"/>
       <c r="C171" s="7"/>
       <c r="D171" s="7"/>
@@ -5295,7 +5399,7 @@
     </row>
     <row r="172" spans="1:8">
       <c r="A172" s="7"/>
-      <c r="B172" s="20"/>
+      <c r="B172" s="7"/>
       <c r="C172" s="7"/>
       <c r="D172" s="7"/>
       <c r="E172" s="7"/>
@@ -5315,7 +5419,7 @@
     </row>
     <row r="174" spans="1:8">
       <c r="A174" s="7"/>
-      <c r="B174" s="7"/>
+      <c r="B174" s="20"/>
       <c r="C174" s="7"/>
       <c r="D174" s="7"/>
       <c r="E174" s="7"/>
@@ -5355,7 +5459,7 @@
     </row>
     <row r="178" spans="1:8">
       <c r="A178" s="7"/>
-      <c r="B178" s="6"/>
+      <c r="B178" s="7"/>
       <c r="C178" s="7"/>
       <c r="D178" s="7"/>
       <c r="E178" s="7"/>
@@ -5365,8 +5469,8 @@
     </row>
     <row r="179" spans="1:8">
       <c r="A179" s="7"/>
-      <c r="B179" s="4"/>
-      <c r="C179" s="4"/>
+      <c r="B179" s="6"/>
+      <c r="C179" s="7"/>
       <c r="D179" s="7"/>
       <c r="E179" s="7"/>
       <c r="F179" s="7"/>
@@ -5375,7 +5479,7 @@
     </row>
     <row r="180" spans="1:8">
       <c r="A180" s="7"/>
-      <c r="B180" s="19"/>
+      <c r="B180" s="4"/>
       <c r="C180" s="4"/>
       <c r="D180" s="7"/>
       <c r="E180" s="7"/>
@@ -5445,7 +5549,7 @@
     </row>
     <row r="187" spans="1:8">
       <c r="A187" s="7"/>
-      <c r="B187" s="4"/>
+      <c r="B187" s="19"/>
       <c r="C187" s="4"/>
       <c r="D187" s="7"/>
       <c r="E187" s="7"/>
@@ -5455,7 +5559,7 @@
     </row>
     <row r="188" spans="1:8">
       <c r="A188" s="7"/>
-      <c r="B188" s="19"/>
+      <c r="B188" s="4"/>
       <c r="C188" s="4"/>
       <c r="D188" s="7"/>
       <c r="E188" s="7"/>
@@ -5465,7 +5569,7 @@
     </row>
     <row r="189" spans="1:8">
       <c r="A189" s="7"/>
-      <c r="B189" s="21"/>
+      <c r="B189" s="19"/>
       <c r="C189" s="4"/>
       <c r="D189" s="7"/>
       <c r="E189" s="7"/>
@@ -5485,7 +5589,7 @@
     </row>
     <row r="191" spans="1:8">
       <c r="A191" s="7"/>
-      <c r="B191" s="19"/>
+      <c r="B191" s="21"/>
       <c r="C191" s="4"/>
       <c r="D191" s="7"/>
       <c r="E191" s="7"/>
@@ -5526,7 +5630,7 @@
     <row r="195" spans="1:8">
       <c r="A195" s="7"/>
       <c r="B195" s="19"/>
-      <c r="C195" s="7"/>
+      <c r="C195" s="4"/>
       <c r="D195" s="7"/>
       <c r="E195" s="7"/>
       <c r="F195" s="7"/>
@@ -5535,7 +5639,7 @@
     </row>
     <row r="196" spans="1:8">
       <c r="A196" s="7"/>
-      <c r="B196" s="4"/>
+      <c r="B196" s="19"/>
       <c r="C196" s="7"/>
       <c r="D196" s="7"/>
       <c r="E196" s="7"/>
@@ -5555,7 +5659,7 @@
     </row>
     <row r="198" spans="1:8">
       <c r="A198" s="7"/>
-      <c r="B198" s="19"/>
+      <c r="B198" s="4"/>
       <c r="C198" s="7"/>
       <c r="D198" s="7"/>
       <c r="E198" s="7"/>
@@ -5615,7 +5719,7 @@
     </row>
     <row r="204" spans="1:8">
       <c r="A204" s="7"/>
-      <c r="B204" s="21"/>
+      <c r="B204" s="19"/>
       <c r="C204" s="7"/>
       <c r="D204" s="7"/>
       <c r="E204" s="7"/>
@@ -5655,7 +5759,7 @@
     </row>
     <row r="208" spans="1:8">
       <c r="A208" s="7"/>
-      <c r="B208" s="4"/>
+      <c r="B208" s="21"/>
       <c r="C208" s="7"/>
       <c r="D208" s="7"/>
       <c r="E208" s="7"/>
@@ -5665,7 +5769,7 @@
     </row>
     <row r="209" spans="1:8">
       <c r="A209" s="7"/>
-      <c r="B209" s="6"/>
+      <c r="B209" s="4"/>
       <c r="C209" s="7"/>
       <c r="D209" s="7"/>
       <c r="E209" s="7"/>
@@ -5675,7 +5779,7 @@
     </row>
     <row r="210" spans="1:8">
       <c r="A210" s="7"/>
-      <c r="B210" s="4"/>
+      <c r="B210" s="6"/>
       <c r="C210" s="7"/>
       <c r="D210" s="7"/>
       <c r="E210" s="7"/>
@@ -5685,7 +5789,7 @@
     </row>
     <row r="211" spans="1:8">
       <c r="A211" s="7"/>
-      <c r="B211" s="19"/>
+      <c r="B211" s="4"/>
       <c r="C211" s="7"/>
       <c r="D211" s="7"/>
       <c r="E211" s="7"/>
@@ -5735,7 +5839,7 @@
     </row>
     <row r="216" spans="1:8">
       <c r="A216" s="7"/>
-      <c r="B216" s="21"/>
+      <c r="B216" s="19"/>
       <c r="C216" s="7"/>
       <c r="D216" s="7"/>
       <c r="E216" s="7"/>
@@ -5745,7 +5849,7 @@
     </row>
     <row r="217" spans="1:8">
       <c r="A217" s="7"/>
-      <c r="B217" s="19"/>
+      <c r="B217" s="21"/>
       <c r="C217" s="7"/>
       <c r="D217" s="7"/>
       <c r="E217" s="7"/>
@@ -5795,7 +5899,7 @@
     </row>
     <row r="222" spans="1:8">
       <c r="A222" s="7"/>
-      <c r="B222" s="21"/>
+      <c r="B222" s="19"/>
       <c r="C222" s="7"/>
       <c r="D222" s="7"/>
       <c r="E222" s="7"/>
@@ -5855,7 +5959,7 @@
     </row>
     <row r="228" spans="1:8">
       <c r="A228" s="7"/>
-      <c r="B228" s="4"/>
+      <c r="B228" s="21"/>
       <c r="C228" s="7"/>
       <c r="D228" s="7"/>
       <c r="E228" s="7"/>
@@ -5865,7 +5969,7 @@
     </row>
     <row r="229" spans="1:8">
       <c r="A229" s="7"/>
-      <c r="B229" s="6"/>
+      <c r="B229" s="4"/>
       <c r="C229" s="7"/>
       <c r="D229" s="7"/>
       <c r="E229" s="7"/>
@@ -5875,8 +5979,8 @@
     </row>
     <row r="230" spans="1:8">
       <c r="A230" s="7"/>
-      <c r="B230" s="4"/>
-      <c r="C230" s="4"/>
+      <c r="B230" s="6"/>
+      <c r="C230" s="7"/>
       <c r="D230" s="7"/>
       <c r="E230" s="7"/>
       <c r="F230" s="7"/>
@@ -5885,7 +5989,7 @@
     </row>
     <row r="231" spans="1:8">
       <c r="A231" s="7"/>
-      <c r="B231" s="19"/>
+      <c r="B231" s="4"/>
       <c r="C231" s="4"/>
       <c r="D231" s="7"/>
       <c r="E231" s="7"/>
@@ -5895,7 +5999,7 @@
     </row>
     <row r="232" spans="1:8">
       <c r="A232" s="7"/>
-      <c r="B232" s="7"/>
+      <c r="B232" s="19"/>
       <c r="C232" s="4"/>
       <c r="D232" s="7"/>
       <c r="E232" s="7"/>
@@ -5905,7 +6009,7 @@
     </row>
     <row r="233" spans="1:8">
       <c r="A233" s="7"/>
-      <c r="B233" s="20"/>
+      <c r="B233" s="7"/>
       <c r="C233" s="4"/>
       <c r="D233" s="7"/>
       <c r="E233" s="7"/>
@@ -5945,7 +6049,7 @@
     </row>
     <row r="237" spans="1:8">
       <c r="A237" s="7"/>
-      <c r="B237" s="7"/>
+      <c r="B237" s="20"/>
       <c r="C237" s="4"/>
       <c r="D237" s="7"/>
       <c r="E237" s="7"/>
@@ -5955,7 +6059,7 @@
     </row>
     <row r="238" spans="1:8">
       <c r="A238" s="7"/>
-      <c r="B238" s="20"/>
+      <c r="B238" s="7"/>
       <c r="C238" s="4"/>
       <c r="D238" s="7"/>
       <c r="E238" s="7"/>
@@ -5965,7 +6069,7 @@
     </row>
     <row r="239" spans="1:8">
       <c r="A239" s="7"/>
-      <c r="B239" s="23"/>
+      <c r="B239" s="20"/>
       <c r="C239" s="4"/>
       <c r="D239" s="7"/>
       <c r="E239" s="7"/>
@@ -5985,7 +6089,7 @@
     </row>
     <row r="241" spans="1:8">
       <c r="A241" s="7"/>
-      <c r="B241" s="20"/>
+      <c r="B241" s="23"/>
       <c r="C241" s="4"/>
       <c r="D241" s="7"/>
       <c r="E241" s="7"/>
@@ -6025,7 +6129,7 @@
     </row>
     <row r="245" spans="1:8">
       <c r="A245" s="7"/>
-      <c r="B245" s="7"/>
+      <c r="B245" s="20"/>
       <c r="C245" s="4"/>
       <c r="D245" s="7"/>
       <c r="E245" s="7"/>
@@ -6035,7 +6139,7 @@
     </row>
     <row r="246" spans="1:8">
       <c r="A246" s="7"/>
-      <c r="B246" s="20"/>
+      <c r="B246" s="7"/>
       <c r="C246" s="4"/>
       <c r="D246" s="7"/>
       <c r="E246" s="7"/>
@@ -6085,7 +6189,7 @@
     </row>
     <row r="251" spans="1:8">
       <c r="A251" s="7"/>
-      <c r="B251" s="7"/>
+      <c r="B251" s="20"/>
       <c r="C251" s="4"/>
       <c r="D251" s="7"/>
       <c r="E251" s="7"/>
@@ -6095,8 +6199,8 @@
     </row>
     <row r="252" spans="1:8">
       <c r="A252" s="7"/>
-      <c r="B252" s="20"/>
-      <c r="C252" s="7"/>
+      <c r="B252" s="7"/>
+      <c r="C252" s="4"/>
       <c r="D252" s="7"/>
       <c r="E252" s="7"/>
       <c r="F252" s="7"/>
@@ -6105,7 +6209,7 @@
     </row>
     <row r="253" spans="1:8">
       <c r="A253" s="7"/>
-      <c r="B253" s="7"/>
+      <c r="B253" s="20"/>
       <c r="C253" s="7"/>
       <c r="D253" s="7"/>
       <c r="E253" s="7"/>
@@ -6115,7 +6219,7 @@
     </row>
     <row r="254" spans="1:8">
       <c r="A254" s="7"/>
-      <c r="B254" s="20"/>
+      <c r="B254" s="7"/>
       <c r="C254" s="7"/>
       <c r="D254" s="7"/>
       <c r="E254" s="7"/>
@@ -6125,7 +6229,7 @@
     </row>
     <row r="255" spans="1:8">
       <c r="A255" s="7"/>
-      <c r="B255" s="23"/>
+      <c r="B255" s="20"/>
       <c r="C255" s="7"/>
       <c r="D255" s="7"/>
       <c r="E255" s="7"/>
@@ -6175,8 +6279,8 @@
     </row>
     <row r="260" spans="1:8">
       <c r="A260" s="7"/>
-      <c r="B260" s="20"/>
-      <c r="C260" s="4"/>
+      <c r="B260" s="23"/>
+      <c r="C260" s="7"/>
       <c r="D260" s="7"/>
       <c r="E260" s="7"/>
       <c r="F260" s="7"/>
@@ -6185,7 +6289,7 @@
     </row>
     <row r="261" spans="1:8">
       <c r="A261" s="7"/>
-      <c r="B261" s="23"/>
+      <c r="B261" s="20"/>
       <c r="C261" s="4"/>
       <c r="D261" s="7"/>
       <c r="E261" s="7"/>
@@ -6195,7 +6299,7 @@
     </row>
     <row r="262" spans="1:8">
       <c r="A262" s="7"/>
-      <c r="B262" s="24"/>
+      <c r="B262" s="23"/>
       <c r="C262" s="4"/>
       <c r="D262" s="7"/>
       <c r="E262" s="7"/>
@@ -6223,9 +6327,9 @@
       <c r="G264" s="30"/>
       <c r="H264" s="7"/>
     </row>
-    <row r="265" spans="1:8" ht="11.25">
+    <row r="265" spans="1:8">
       <c r="A265" s="7"/>
-      <c r="B265" s="25"/>
+      <c r="B265" s="24"/>
       <c r="C265" s="4"/>
       <c r="D265" s="7"/>
       <c r="E265" s="7"/>
@@ -6233,9 +6337,9 @@
       <c r="G265" s="30"/>
       <c r="H265" s="7"/>
     </row>
-    <row r="266" spans="1:8">
+    <row r="266" spans="1:8" ht="11.25">
       <c r="A266" s="7"/>
-      <c r="B266" s="23"/>
+      <c r="B266" s="25"/>
       <c r="C266" s="4"/>
       <c r="D266" s="7"/>
       <c r="E266" s="7"/>
@@ -6275,7 +6379,7 @@
     </row>
     <row r="270" spans="1:8">
       <c r="A270" s="7"/>
-      <c r="B270" s="24"/>
+      <c r="B270" s="23"/>
       <c r="C270" s="4"/>
       <c r="D270" s="7"/>
       <c r="E270" s="7"/>
@@ -6305,7 +6409,7 @@
     </row>
     <row r="273" spans="1:8">
       <c r="A273" s="7"/>
-      <c r="B273" s="23"/>
+      <c r="B273" s="24"/>
       <c r="C273" s="4"/>
       <c r="D273" s="7"/>
       <c r="E273" s="7"/>
@@ -6315,7 +6419,7 @@
     </row>
     <row r="274" spans="1:8">
       <c r="A274" s="7"/>
-      <c r="B274" s="24"/>
+      <c r="B274" s="23"/>
       <c r="C274" s="4"/>
       <c r="D274" s="7"/>
       <c r="E274" s="7"/>
@@ -6323,15 +6427,15 @@
       <c r="G274" s="30"/>
       <c r="H274" s="7"/>
     </row>
-    <row r="275" spans="1:8" s="2" customFormat="1">
-      <c r="A275" s="4"/>
+    <row r="275" spans="1:8">
+      <c r="A275" s="7"/>
       <c r="B275" s="24"/>
       <c r="C275" s="4"/>
-      <c r="D275" s="4"/>
-      <c r="E275" s="4"/>
-      <c r="F275" s="4"/>
-      <c r="G275" s="34"/>
-      <c r="H275" s="4"/>
+      <c r="D275" s="7"/>
+      <c r="E275" s="7"/>
+      <c r="F275" s="7"/>
+      <c r="G275" s="30"/>
+      <c r="H275" s="7"/>
     </row>
     <row r="276" spans="1:8" s="2" customFormat="1">
       <c r="A276" s="4"/>
@@ -6343,19 +6447,19 @@
       <c r="G276" s="34"/>
       <c r="H276" s="4"/>
     </row>
-    <row r="277" spans="1:8">
-      <c r="A277" s="7"/>
+    <row r="277" spans="1:8" s="2" customFormat="1">
+      <c r="A277" s="4"/>
       <c r="B277" s="24"/>
       <c r="C277" s="4"/>
-      <c r="D277" s="7"/>
-      <c r="E277" s="7"/>
-      <c r="F277" s="7"/>
-      <c r="G277" s="30"/>
-      <c r="H277" s="7"/>
+      <c r="D277" s="4"/>
+      <c r="E277" s="4"/>
+      <c r="F277" s="4"/>
+      <c r="G277" s="34"/>
+      <c r="H277" s="4"/>
     </row>
     <row r="278" spans="1:8">
       <c r="A278" s="7"/>
-      <c r="B278" s="23"/>
+      <c r="B278" s="24"/>
       <c r="C278" s="4"/>
       <c r="D278" s="7"/>
       <c r="E278" s="7"/>
@@ -6365,7 +6469,7 @@
     </row>
     <row r="279" spans="1:8">
       <c r="A279" s="7"/>
-      <c r="B279" s="24"/>
+      <c r="B279" s="23"/>
       <c r="C279" s="4"/>
       <c r="D279" s="7"/>
       <c r="E279" s="7"/>
@@ -6395,7 +6499,7 @@
     </row>
     <row r="282" spans="1:8">
       <c r="A282" s="7"/>
-      <c r="B282" s="22"/>
+      <c r="B282" s="24"/>
       <c r="C282" s="4"/>
       <c r="D282" s="7"/>
       <c r="E282" s="7"/>
@@ -6405,7 +6509,7 @@
     </row>
     <row r="283" spans="1:8">
       <c r="A283" s="7"/>
-      <c r="B283" s="7"/>
+      <c r="B283" s="22"/>
       <c r="C283" s="4"/>
       <c r="D283" s="7"/>
       <c r="E283" s="7"/>
@@ -6425,7 +6529,7 @@
     </row>
     <row r="285" spans="1:8">
       <c r="A285" s="7"/>
-      <c r="B285" s="20"/>
+      <c r="B285" s="7"/>
       <c r="C285" s="4"/>
       <c r="D285" s="7"/>
       <c r="E285" s="7"/>
@@ -6445,7 +6549,7 @@
     </row>
     <row r="287" spans="1:8">
       <c r="A287" s="7"/>
-      <c r="B287" s="7"/>
+      <c r="B287" s="20"/>
       <c r="C287" s="4"/>
       <c r="D287" s="7"/>
       <c r="E287" s="7"/>
@@ -6476,7 +6580,7 @@
     <row r="290" spans="1:8">
       <c r="A290" s="7"/>
       <c r="B290" s="7"/>
-      <c r="C290" s="7"/>
+      <c r="C290" s="4"/>
       <c r="D290" s="7"/>
       <c r="E290" s="7"/>
       <c r="F290" s="7"/>
@@ -6485,7 +6589,7 @@
     </row>
     <row r="291" spans="1:8">
       <c r="A291" s="7"/>
-      <c r="B291" s="6"/>
+      <c r="B291" s="7"/>
       <c r="C291" s="7"/>
       <c r="D291" s="7"/>
       <c r="E291" s="7"/>
@@ -6495,7 +6599,7 @@
     </row>
     <row r="292" spans="1:8">
       <c r="A292" s="7"/>
-      <c r="B292" s="7"/>
+      <c r="B292" s="6"/>
       <c r="C292" s="7"/>
       <c r="D292" s="7"/>
       <c r="E292" s="7"/>
@@ -6575,7 +6679,7 @@
     </row>
     <row r="300" spans="1:8">
       <c r="A300" s="7"/>
-      <c r="B300" s="6"/>
+      <c r="B300" s="7"/>
       <c r="C300" s="7"/>
       <c r="D300" s="7"/>
       <c r="E300" s="7"/>
@@ -6585,8 +6689,8 @@
     </row>
     <row r="301" spans="1:8">
       <c r="A301" s="7"/>
-      <c r="B301" s="4"/>
-      <c r="C301" s="4"/>
+      <c r="B301" s="6"/>
+      <c r="C301" s="7"/>
       <c r="D301" s="7"/>
       <c r="E301" s="7"/>
       <c r="F301" s="7"/>
@@ -6595,7 +6699,7 @@
     </row>
     <row r="302" spans="1:8">
       <c r="A302" s="7"/>
-      <c r="B302" s="19"/>
+      <c r="B302" s="4"/>
       <c r="C302" s="4"/>
       <c r="D302" s="7"/>
       <c r="E302" s="7"/>
@@ -6625,7 +6729,7 @@
     </row>
     <row r="305" spans="1:8">
       <c r="A305" s="7"/>
-      <c r="B305" s="4"/>
+      <c r="B305" s="19"/>
       <c r="C305" s="4"/>
       <c r="D305" s="7"/>
       <c r="E305" s="7"/>
@@ -6685,7 +6789,7 @@
     </row>
     <row r="311" spans="1:8">
       <c r="A311" s="7"/>
-      <c r="B311" s="19"/>
+      <c r="B311" s="4"/>
       <c r="C311" s="4"/>
       <c r="D311" s="7"/>
       <c r="E311" s="7"/>
@@ -6705,7 +6809,7 @@
     </row>
     <row r="313" spans="1:8">
       <c r="A313" s="7"/>
-      <c r="B313" s="21"/>
+      <c r="B313" s="19"/>
       <c r="C313" s="4"/>
       <c r="D313" s="7"/>
       <c r="E313" s="7"/>
@@ -6715,8 +6819,8 @@
     </row>
     <row r="314" spans="1:8">
       <c r="A314" s="7"/>
-      <c r="B314" s="7"/>
-      <c r="C314" s="7"/>
+      <c r="B314" s="21"/>
+      <c r="C314" s="4"/>
       <c r="D314" s="7"/>
       <c r="E314" s="7"/>
       <c r="F314" s="7"/>
@@ -6725,7 +6829,7 @@
     </row>
     <row r="315" spans="1:8">
       <c r="A315" s="7"/>
-      <c r="B315" s="6"/>
+      <c r="B315" s="7"/>
       <c r="C315" s="7"/>
       <c r="D315" s="7"/>
       <c r="E315" s="7"/>
@@ -6733,15 +6837,15 @@
       <c r="G315" s="30"/>
       <c r="H315" s="7"/>
     </row>
-    <row r="316" spans="1:8" s="2" customFormat="1">
-      <c r="A316" s="4"/>
-      <c r="B316" s="4"/>
-      <c r="C316" s="9"/>
-      <c r="D316" s="4"/>
-      <c r="E316" s="4"/>
-      <c r="F316" s="4"/>
-      <c r="G316" s="34"/>
-      <c r="H316" s="4"/>
+    <row r="316" spans="1:8">
+      <c r="A316" s="7"/>
+      <c r="B316" s="6"/>
+      <c r="C316" s="7"/>
+      <c r="D316" s="7"/>
+      <c r="E316" s="7"/>
+      <c r="F316" s="7"/>
+      <c r="G316" s="30"/>
+      <c r="H316" s="7"/>
     </row>
     <row r="317" spans="1:8" s="2" customFormat="1">
       <c r="A317" s="4"/>
@@ -6765,7 +6869,7 @@
     </row>
     <row r="319" spans="1:8" s="2" customFormat="1">
       <c r="A319" s="4"/>
-      <c r="B319" s="19"/>
+      <c r="B319" s="4"/>
       <c r="C319" s="9"/>
       <c r="D319" s="4"/>
       <c r="E319" s="4"/>
@@ -6815,8 +6919,8 @@
     </row>
     <row r="324" spans="1:8" s="2" customFormat="1">
       <c r="A324" s="4"/>
-      <c r="B324" s="26"/>
-      <c r="C324" s="4"/>
+      <c r="B324" s="19"/>
+      <c r="C324" s="9"/>
       <c r="D324" s="4"/>
       <c r="E324" s="4"/>
       <c r="F324" s="4"/>
@@ -6865,7 +6969,7 @@
     </row>
     <row r="329" spans="1:8" s="2" customFormat="1">
       <c r="A329" s="4"/>
-      <c r="B329" s="21"/>
+      <c r="B329" s="26"/>
       <c r="C329" s="4"/>
       <c r="D329" s="4"/>
       <c r="E329" s="4"/>
@@ -6915,7 +7019,7 @@
     </row>
     <row r="334" spans="1:8" s="2" customFormat="1">
       <c r="A334" s="4"/>
-      <c r="B334" s="19"/>
+      <c r="B334" s="21"/>
       <c r="C334" s="4"/>
       <c r="D334" s="4"/>
       <c r="E334" s="4"/>
@@ -6925,7 +7029,7 @@
     </row>
     <row r="335" spans="1:8" s="2" customFormat="1">
       <c r="A335" s="4"/>
-      <c r="B335" s="21"/>
+      <c r="B335" s="19"/>
       <c r="C335" s="4"/>
       <c r="D335" s="4"/>
       <c r="E335" s="4"/>
@@ -6935,7 +7039,7 @@
     </row>
     <row r="336" spans="1:8" s="2" customFormat="1">
       <c r="A336" s="4"/>
-      <c r="B336" s="4"/>
+      <c r="B336" s="21"/>
       <c r="C336" s="4"/>
       <c r="D336" s="4"/>
       <c r="E336" s="4"/>
@@ -6943,20 +7047,20 @@
       <c r="G336" s="34"/>
       <c r="H336" s="4"/>
     </row>
-    <row r="337" spans="1:8">
-      <c r="A337" s="7"/>
-      <c r="B337" s="6"/>
-      <c r="C337" s="7"/>
-      <c r="D337" s="7"/>
-      <c r="E337" s="7"/>
-      <c r="F337" s="7"/>
-      <c r="G337" s="30"/>
-      <c r="H337" s="7"/>
+    <row r="337" spans="1:8" s="2" customFormat="1">
+      <c r="A337" s="4"/>
+      <c r="B337" s="4"/>
+      <c r="C337" s="4"/>
+      <c r="D337" s="4"/>
+      <c r="E337" s="4"/>
+      <c r="F337" s="4"/>
+      <c r="G337" s="34"/>
+      <c r="H337" s="4"/>
     </row>
     <row r="338" spans="1:8">
       <c r="A338" s="7"/>
-      <c r="B338" s="7"/>
-      <c r="C338" s="4"/>
+      <c r="B338" s="6"/>
+      <c r="C338" s="7"/>
       <c r="D338" s="7"/>
       <c r="E338" s="7"/>
       <c r="F338" s="7"/>
@@ -7025,7 +7129,7 @@
     </row>
     <row r="345" spans="1:8">
       <c r="A345" s="7"/>
-      <c r="B345" s="4"/>
+      <c r="B345" s="7"/>
       <c r="C345" s="4"/>
       <c r="D345" s="7"/>
       <c r="E345" s="7"/>
@@ -7036,7 +7140,7 @@
     <row r="346" spans="1:8">
       <c r="A346" s="7"/>
       <c r="B346" s="4"/>
-      <c r="C346" s="7"/>
+      <c r="C346" s="4"/>
       <c r="D346" s="7"/>
       <c r="E346" s="7"/>
       <c r="F346" s="7"/>
@@ -7045,7 +7149,7 @@
     </row>
     <row r="347" spans="1:8">
       <c r="A347" s="7"/>
-      <c r="B347" s="6"/>
+      <c r="B347" s="4"/>
       <c r="C347" s="7"/>
       <c r="D347" s="7"/>
       <c r="E347" s="7"/>
@@ -7055,7 +7159,7 @@
     </row>
     <row r="348" spans="1:8">
       <c r="A348" s="7"/>
-      <c r="B348" s="7"/>
+      <c r="B348" s="6"/>
       <c r="C348" s="7"/>
       <c r="D348" s="7"/>
       <c r="E348" s="7"/>
@@ -7065,7 +7169,7 @@
     </row>
     <row r="349" spans="1:8">
       <c r="A349" s="7"/>
-      <c r="B349" s="22"/>
+      <c r="B349" s="7"/>
       <c r="C349" s="7"/>
       <c r="D349" s="7"/>
       <c r="E349" s="7"/>
@@ -7075,7 +7179,7 @@
     </row>
     <row r="350" spans="1:8">
       <c r="A350" s="7"/>
-      <c r="B350" s="7"/>
+      <c r="B350" s="22"/>
       <c r="C350" s="7"/>
       <c r="D350" s="7"/>
       <c r="E350" s="7"/>
@@ -7115,7 +7219,7 @@
     </row>
     <row r="354" spans="1:8">
       <c r="A354" s="7"/>
-      <c r="B354" s="6"/>
+      <c r="B354" s="7"/>
       <c r="C354" s="7"/>
       <c r="D354" s="7"/>
       <c r="E354" s="7"/>
@@ -7125,7 +7229,7 @@
     </row>
     <row r="355" spans="1:8">
       <c r="A355" s="7"/>
-      <c r="B355" s="7"/>
+      <c r="B355" s="6"/>
       <c r="C355" s="7"/>
       <c r="D355" s="7"/>
       <c r="E355" s="7"/>
@@ -7135,7 +7239,7 @@
     </row>
     <row r="356" spans="1:8">
       <c r="A356" s="7"/>
-      <c r="B356" s="20"/>
+      <c r="B356" s="7"/>
       <c r="C356" s="7"/>
       <c r="D356" s="7"/>
       <c r="E356" s="7"/>
@@ -7165,7 +7269,7 @@
     </row>
     <row r="359" spans="1:8">
       <c r="A359" s="7"/>
-      <c r="B359" s="22"/>
+      <c r="B359" s="20"/>
       <c r="C359" s="7"/>
       <c r="D359" s="7"/>
       <c r="E359" s="7"/>
@@ -7175,7 +7279,7 @@
     </row>
     <row r="360" spans="1:8">
       <c r="A360" s="7"/>
-      <c r="B360" s="20"/>
+      <c r="B360" s="22"/>
       <c r="C360" s="7"/>
       <c r="D360" s="7"/>
       <c r="E360" s="7"/>
@@ -7195,7 +7299,7 @@
     </row>
     <row r="362" spans="1:8">
       <c r="A362" s="7"/>
-      <c r="B362" s="22"/>
+      <c r="B362" s="20"/>
       <c r="C362" s="7"/>
       <c r="D362" s="7"/>
       <c r="E362" s="7"/>
@@ -7205,7 +7309,7 @@
     </row>
     <row r="363" spans="1:8">
       <c r="A363" s="7"/>
-      <c r="B363" s="20"/>
+      <c r="B363" s="22"/>
       <c r="C363" s="7"/>
       <c r="D363" s="7"/>
       <c r="E363" s="7"/>
@@ -7215,7 +7319,7 @@
     </row>
     <row r="364" spans="1:8">
       <c r="A364" s="7"/>
-      <c r="B364" s="22"/>
+      <c r="B364" s="20"/>
       <c r="C364" s="7"/>
       <c r="D364" s="7"/>
       <c r="E364" s="7"/>
@@ -7225,7 +7329,7 @@
     </row>
     <row r="365" spans="1:8">
       <c r="A365" s="7"/>
-      <c r="B365" s="20"/>
+      <c r="B365" s="22"/>
       <c r="C365" s="7"/>
       <c r="D365" s="7"/>
       <c r="E365" s="7"/>
@@ -7255,7 +7359,7 @@
     </row>
     <row r="368" spans="1:8">
       <c r="A368" s="7"/>
-      <c r="B368" s="7"/>
+      <c r="B368" s="20"/>
       <c r="C368" s="7"/>
       <c r="D368" s="7"/>
       <c r="E368" s="7"/>
@@ -7265,7 +7369,7 @@
     </row>
     <row r="369" spans="1:8">
       <c r="A369" s="7"/>
-      <c r="B369" s="27"/>
+      <c r="B369" s="7"/>
       <c r="C369" s="7"/>
       <c r="D369" s="7"/>
       <c r="E369" s="7"/>
@@ -7275,7 +7379,7 @@
     </row>
     <row r="370" spans="1:8">
       <c r="A370" s="7"/>
-      <c r="B370" s="22"/>
+      <c r="B370" s="27"/>
       <c r="C370" s="7"/>
       <c r="D370" s="7"/>
       <c r="E370" s="7"/>
@@ -7285,8 +7389,8 @@
     </row>
     <row r="371" spans="1:8">
       <c r="A371" s="7"/>
-      <c r="B371" s="7"/>
-      <c r="C371" s="4"/>
+      <c r="B371" s="22"/>
+      <c r="C371" s="7"/>
       <c r="D371" s="7"/>
       <c r="E371" s="7"/>
       <c r="F371" s="7"/>
@@ -7295,7 +7399,7 @@
     </row>
     <row r="372" spans="1:8">
       <c r="A372" s="7"/>
-      <c r="B372" s="20"/>
+      <c r="B372" s="7"/>
       <c r="C372" s="4"/>
       <c r="D372" s="7"/>
       <c r="E372" s="7"/>
@@ -7325,7 +7429,7 @@
     </row>
     <row r="375" spans="1:8">
       <c r="A375" s="7"/>
-      <c r="B375" s="7"/>
+      <c r="B375" s="20"/>
       <c r="C375" s="4"/>
       <c r="D375" s="7"/>
       <c r="E375" s="7"/>
@@ -7355,7 +7459,7 @@
     </row>
     <row r="378" spans="1:8">
       <c r="A378" s="7"/>
-      <c r="B378" s="20"/>
+      <c r="B378" s="7"/>
       <c r="C378" s="4"/>
       <c r="D378" s="7"/>
       <c r="E378" s="7"/>
@@ -7375,8 +7479,8 @@
     </row>
     <row r="380" spans="1:8">
       <c r="A380" s="7"/>
-      <c r="B380" s="7"/>
-      <c r="C380" s="7"/>
+      <c r="B380" s="20"/>
+      <c r="C380" s="4"/>
       <c r="D380" s="7"/>
       <c r="E380" s="7"/>
       <c r="F380" s="7"/>
@@ -7385,7 +7489,7 @@
     </row>
     <row r="381" spans="1:8">
       <c r="A381" s="7"/>
-      <c r="B381" s="6"/>
+      <c r="B381" s="7"/>
       <c r="C381" s="7"/>
       <c r="D381" s="7"/>
       <c r="E381" s="7"/>
@@ -7395,7 +7499,7 @@
     </row>
     <row r="382" spans="1:8">
       <c r="A382" s="7"/>
-      <c r="B382" s="7"/>
+      <c r="B382" s="6"/>
       <c r="C382" s="7"/>
       <c r="D382" s="7"/>
       <c r="E382" s="7"/>
@@ -7455,7 +7559,7 @@
     </row>
     <row r="388" spans="1:8">
       <c r="A388" s="7"/>
-      <c r="B388" s="6"/>
+      <c r="B388" s="7"/>
       <c r="C388" s="7"/>
       <c r="D388" s="7"/>
       <c r="E388" s="7"/>
@@ -7465,7 +7569,7 @@
     </row>
     <row r="389" spans="1:8">
       <c r="A389" s="7"/>
-      <c r="B389" s="7"/>
+      <c r="B389" s="6"/>
       <c r="C389" s="7"/>
       <c r="D389" s="7"/>
       <c r="E389" s="7"/>
@@ -7486,7 +7590,7 @@
     <row r="391" spans="1:8">
       <c r="A391" s="7"/>
       <c r="B391" s="7"/>
-      <c r="C391" s="4"/>
+      <c r="C391" s="7"/>
       <c r="D391" s="7"/>
       <c r="E391" s="7"/>
       <c r="F391" s="7"/>
@@ -7495,7 +7599,7 @@
     </row>
     <row r="392" spans="1:8">
       <c r="A392" s="7"/>
-      <c r="B392" s="20"/>
+      <c r="B392" s="7"/>
       <c r="C392" s="4"/>
       <c r="D392" s="7"/>
       <c r="E392" s="7"/>
@@ -7506,7 +7610,7 @@
     <row r="393" spans="1:8">
       <c r="A393" s="7"/>
       <c r="B393" s="20"/>
-      <c r="C393" s="7"/>
+      <c r="C393" s="4"/>
       <c r="D393" s="7"/>
       <c r="E393" s="7"/>
       <c r="F393" s="7"/>
@@ -7515,7 +7619,7 @@
     </row>
     <row r="394" spans="1:8">
       <c r="A394" s="7"/>
-      <c r="B394" s="27"/>
+      <c r="B394" s="20"/>
       <c r="C394" s="7"/>
       <c r="D394" s="7"/>
       <c r="E394" s="7"/>
@@ -7525,7 +7629,7 @@
     </row>
     <row r="395" spans="1:8">
       <c r="A395" s="7"/>
-      <c r="B395" s="22"/>
+      <c r="B395" s="27"/>
       <c r="C395" s="7"/>
       <c r="D395" s="7"/>
       <c r="E395" s="7"/>
@@ -7575,7 +7679,7 @@
     </row>
     <row r="400" spans="1:8">
       <c r="A400" s="7"/>
-      <c r="B400" s="7"/>
+      <c r="B400" s="22"/>
       <c r="C400" s="7"/>
       <c r="D400" s="7"/>
       <c r="E400" s="7"/>
@@ -7585,7 +7689,7 @@
     </row>
     <row r="401" spans="1:8">
       <c r="A401" s="7"/>
-      <c r="B401" s="6"/>
+      <c r="B401" s="7"/>
       <c r="C401" s="7"/>
       <c r="D401" s="7"/>
       <c r="E401" s="7"/>
@@ -7595,7 +7699,7 @@
     </row>
     <row r="402" spans="1:8">
       <c r="A402" s="7"/>
-      <c r="B402" s="7"/>
+      <c r="B402" s="6"/>
       <c r="C402" s="7"/>
       <c r="D402" s="7"/>
       <c r="E402" s="7"/>
@@ -7605,7 +7709,7 @@
     </row>
     <row r="403" spans="1:8">
       <c r="A403" s="7"/>
-      <c r="B403" s="20"/>
+      <c r="B403" s="7"/>
       <c r="C403" s="7"/>
       <c r="D403" s="7"/>
       <c r="E403" s="7"/>
@@ -7615,7 +7719,7 @@
     </row>
     <row r="404" spans="1:8">
       <c r="A404" s="7"/>
-      <c r="B404" s="22"/>
+      <c r="B404" s="20"/>
       <c r="C404" s="7"/>
       <c r="D404" s="7"/>
       <c r="E404" s="7"/>
@@ -7635,7 +7739,7 @@
     </row>
     <row r="406" spans="1:8">
       <c r="A406" s="7"/>
-      <c r="B406" s="20"/>
+      <c r="B406" s="22"/>
       <c r="C406" s="7"/>
       <c r="D406" s="7"/>
       <c r="E406" s="7"/>
@@ -7675,7 +7779,7 @@
     </row>
     <row r="410" spans="1:8">
       <c r="A410" s="7"/>
-      <c r="B410" s="7"/>
+      <c r="B410" s="20"/>
       <c r="C410" s="7"/>
       <c r="D410" s="7"/>
       <c r="E410" s="7"/>
@@ -7685,7 +7789,7 @@
     </row>
     <row r="411" spans="1:8">
       <c r="A411" s="7"/>
-      <c r="B411" s="20"/>
+      <c r="B411" s="7"/>
       <c r="C411" s="7"/>
       <c r="D411" s="7"/>
       <c r="E411" s="7"/>
@@ -7705,7 +7809,7 @@
     </row>
     <row r="413" spans="1:8">
       <c r="A413" s="7"/>
-      <c r="B413" s="22"/>
+      <c r="B413" s="20"/>
       <c r="C413" s="7"/>
       <c r="D413" s="7"/>
       <c r="E413" s="7"/>
@@ -7715,7 +7819,7 @@
     </row>
     <row r="414" spans="1:8">
       <c r="A414" s="7"/>
-      <c r="B414" s="7"/>
+      <c r="B414" s="22"/>
       <c r="C414" s="7"/>
       <c r="D414" s="7"/>
       <c r="E414" s="7"/>
@@ -7725,7 +7829,7 @@
     </row>
     <row r="415" spans="1:8">
       <c r="A415" s="7"/>
-      <c r="B415" s="6"/>
+      <c r="B415" s="7"/>
       <c r="C415" s="7"/>
       <c r="D415" s="7"/>
       <c r="E415" s="7"/>
@@ -7735,7 +7839,7 @@
     </row>
     <row r="416" spans="1:8">
       <c r="A416" s="7"/>
-      <c r="B416" s="7"/>
+      <c r="B416" s="6"/>
       <c r="C416" s="7"/>
       <c r="D416" s="7"/>
       <c r="E416" s="7"/>
@@ -7755,7 +7859,7 @@
     </row>
     <row r="418" spans="1:8">
       <c r="A418" s="7"/>
-      <c r="B418" s="6"/>
+      <c r="B418" s="7"/>
       <c r="C418" s="7"/>
       <c r="D418" s="7"/>
       <c r="E418" s="7"/>
@@ -7765,7 +7869,7 @@
     </row>
     <row r="419" spans="1:8">
       <c r="A419" s="7"/>
-      <c r="B419" s="7"/>
+      <c r="B419" s="6"/>
       <c r="C419" s="7"/>
       <c r="D419" s="7"/>
       <c r="E419" s="7"/>
@@ -7775,7 +7879,7 @@
     </row>
     <row r="420" spans="1:8">
       <c r="A420" s="7"/>
-      <c r="B420" s="20"/>
+      <c r="B420" s="7"/>
       <c r="C420" s="7"/>
       <c r="D420" s="7"/>
       <c r="E420" s="7"/>
@@ -7795,7 +7899,7 @@
     </row>
     <row r="422" spans="1:8">
       <c r="A422" s="7"/>
-      <c r="B422" s="7"/>
+      <c r="B422" s="20"/>
       <c r="C422" s="7"/>
       <c r="D422" s="7"/>
       <c r="E422" s="7"/>
@@ -7805,7 +7909,7 @@
     </row>
     <row r="423" spans="1:8">
       <c r="A423" s="7"/>
-      <c r="B423" s="6"/>
+      <c r="B423" s="7"/>
       <c r="C423" s="7"/>
       <c r="D423" s="7"/>
       <c r="E423" s="7"/>
@@ -7815,7 +7919,7 @@
     </row>
     <row r="424" spans="1:8">
       <c r="A424" s="7"/>
-      <c r="B424" s="7"/>
+      <c r="B424" s="6"/>
       <c r="C424" s="7"/>
       <c r="D424" s="7"/>
       <c r="E424" s="7"/>
@@ -7865,7 +7969,7 @@
     </row>
     <row r="429" spans="1:8">
       <c r="A429" s="7"/>
-      <c r="B429" s="6"/>
+      <c r="B429" s="7"/>
       <c r="C429" s="7"/>
       <c r="D429" s="7"/>
       <c r="E429" s="7"/>
@@ -7875,7 +7979,7 @@
     </row>
     <row r="430" spans="1:8">
       <c r="A430" s="7"/>
-      <c r="B430" s="7"/>
+      <c r="B430" s="6"/>
       <c r="C430" s="7"/>
       <c r="D430" s="7"/>
       <c r="E430" s="7"/>
@@ -7935,7 +8039,7 @@
     </row>
     <row r="436" spans="1:8">
       <c r="A436" s="7"/>
-      <c r="B436" s="6"/>
+      <c r="B436" s="7"/>
       <c r="C436" s="7"/>
       <c r="D436" s="7"/>
       <c r="E436" s="7"/>
@@ -7945,7 +8049,7 @@
     </row>
     <row r="437" spans="1:8">
       <c r="A437" s="7"/>
-      <c r="B437" s="7"/>
+      <c r="B437" s="6"/>
       <c r="C437" s="7"/>
       <c r="D437" s="7"/>
       <c r="E437" s="7"/>
@@ -7965,7 +8069,7 @@
     </row>
     <row r="439" spans="1:8">
       <c r="A439" s="7"/>
-      <c r="B439" s="6"/>
+      <c r="B439" s="7"/>
       <c r="C439" s="7"/>
       <c r="D439" s="7"/>
       <c r="E439" s="7"/>
@@ -7975,7 +8079,7 @@
     </row>
     <row r="440" spans="1:8">
       <c r="A440" s="7"/>
-      <c r="B440" s="4"/>
+      <c r="B440" s="6"/>
       <c r="C440" s="7"/>
       <c r="D440" s="7"/>
       <c r="E440" s="7"/>
@@ -7995,7 +8099,7 @@
     </row>
     <row r="442" spans="1:8">
       <c r="A442" s="7"/>
-      <c r="B442" s="7"/>
+      <c r="B442" s="4"/>
       <c r="C442" s="7"/>
       <c r="D442" s="7"/>
       <c r="E442" s="7"/>
@@ -8025,7 +8129,7 @@
     </row>
     <row r="445" spans="1:8">
       <c r="A445" s="7"/>
-      <c r="B445" s="6"/>
+      <c r="B445" s="7"/>
       <c r="C445" s="7"/>
       <c r="D445" s="7"/>
       <c r="E445" s="7"/>
@@ -8035,8 +8139,8 @@
     </row>
     <row r="446" spans="1:8">
       <c r="A446" s="7"/>
-      <c r="B446" s="7"/>
-      <c r="C446" s="4"/>
+      <c r="B446" s="6"/>
+      <c r="C446" s="7"/>
       <c r="D446" s="7"/>
       <c r="E446" s="7"/>
       <c r="F446" s="7"/>
@@ -8086,7 +8190,7 @@
     <row r="451" spans="1:8">
       <c r="A451" s="7"/>
       <c r="B451" s="7"/>
-      <c r="C451" s="7"/>
+      <c r="C451" s="4"/>
       <c r="D451" s="7"/>
       <c r="E451" s="7"/>
       <c r="F451" s="7"/>
@@ -8095,7 +8199,7 @@
     </row>
     <row r="452" spans="1:8">
       <c r="A452" s="7"/>
-      <c r="B452" s="6"/>
+      <c r="B452" s="7"/>
       <c r="C452" s="7"/>
       <c r="D452" s="7"/>
       <c r="E452" s="7"/>
@@ -8105,8 +8209,8 @@
     </row>
     <row r="453" spans="1:8">
       <c r="A453" s="7"/>
-      <c r="B453" s="7"/>
-      <c r="C453" s="4"/>
+      <c r="B453" s="6"/>
+      <c r="C453" s="7"/>
       <c r="D453" s="7"/>
       <c r="E453" s="7"/>
       <c r="F453" s="7"/>
@@ -8146,7 +8250,7 @@
     <row r="457" spans="1:8">
       <c r="A457" s="7"/>
       <c r="B457" s="7"/>
-      <c r="C457" s="7"/>
+      <c r="C457" s="4"/>
       <c r="D457" s="7"/>
       <c r="E457" s="7"/>
       <c r="F457" s="7"/>
@@ -8155,7 +8259,7 @@
     </row>
     <row r="458" spans="1:8">
       <c r="A458" s="7"/>
-      <c r="B458" s="6"/>
+      <c r="B458" s="7"/>
       <c r="C458" s="7"/>
       <c r="D458" s="7"/>
       <c r="E458" s="7"/>
@@ -8165,7 +8269,7 @@
     </row>
     <row r="459" spans="1:8">
       <c r="A459" s="7"/>
-      <c r="B459" s="22"/>
+      <c r="B459" s="6"/>
       <c r="C459" s="7"/>
       <c r="D459" s="7"/>
       <c r="E459" s="7"/>
@@ -8225,7 +8329,7 @@
     </row>
     <row r="465" spans="1:8">
       <c r="A465" s="7"/>
-      <c r="B465" s="7"/>
+      <c r="B465" s="22"/>
       <c r="C465" s="7"/>
       <c r="D465" s="7"/>
       <c r="E465" s="7"/>
@@ -8235,7 +8339,7 @@
     </row>
     <row r="466" spans="1:8">
       <c r="A466" s="7"/>
-      <c r="B466" s="6"/>
+      <c r="B466" s="7"/>
       <c r="C466" s="7"/>
       <c r="D466" s="7"/>
       <c r="E466" s="7"/>
@@ -8245,7 +8349,7 @@
     </row>
     <row r="467" spans="1:8">
       <c r="A467" s="7"/>
-      <c r="B467" s="22"/>
+      <c r="B467" s="6"/>
       <c r="C467" s="7"/>
       <c r="D467" s="7"/>
       <c r="E467" s="7"/>
@@ -8274,8 +8378,8 @@
       <c r="H469" s="7"/>
     </row>
     <row r="470" spans="1:8">
-      <c r="A470" s="6"/>
-      <c r="B470" s="7"/>
+      <c r="A470" s="7"/>
+      <c r="B470" s="22"/>
       <c r="C470" s="7"/>
       <c r="D470" s="7"/>
       <c r="E470" s="7"/>
@@ -8284,7 +8388,7 @@
       <c r="H470" s="7"/>
     </row>
     <row r="471" spans="1:8">
-      <c r="A471" s="7"/>
+      <c r="A471" s="6"/>
       <c r="B471" s="7"/>
       <c r="C471" s="7"/>
       <c r="D471" s="7"/>
@@ -8325,7 +8429,7 @@
     </row>
     <row r="475" spans="1:8">
       <c r="A475" s="7"/>
-      <c r="B475" s="28"/>
+      <c r="B475" s="7"/>
       <c r="C475" s="7"/>
       <c r="D475" s="7"/>
       <c r="E475" s="7"/>
@@ -8355,7 +8459,7 @@
     </row>
     <row r="478" spans="1:8">
       <c r="A478" s="7"/>
-      <c r="B478" s="7"/>
+      <c r="B478" s="28"/>
       <c r="C478" s="7"/>
       <c r="D478" s="7"/>
       <c r="E478" s="7"/>
@@ -8365,7 +8469,7 @@
     </row>
     <row r="479" spans="1:8">
       <c r="A479" s="7"/>
-      <c r="B479" s="28"/>
+      <c r="B479" s="7"/>
       <c r="C479" s="7"/>
       <c r="D479" s="7"/>
       <c r="E479" s="7"/>
@@ -8375,7 +8479,7 @@
     </row>
     <row r="480" spans="1:8">
       <c r="A480" s="7"/>
-      <c r="B480" s="7"/>
+      <c r="B480" s="28"/>
       <c r="C480" s="7"/>
       <c r="D480" s="7"/>
       <c r="E480" s="7"/>
@@ -8385,21 +8489,21 @@
     </row>
     <row r="481" spans="1:8">
       <c r="A481" s="7"/>
-      <c r="B481" s="29"/>
-      <c r="C481" s="30"/>
+      <c r="B481" s="7"/>
+      <c r="C481" s="7"/>
       <c r="D481" s="7"/>
       <c r="E481" s="7"/>
-      <c r="F481" s="29"/>
+      <c r="F481" s="7"/>
       <c r="G481" s="30"/>
       <c r="H481" s="7"/>
     </row>
     <row r="482" spans="1:8">
       <c r="A482" s="7"/>
-      <c r="B482" s="7"/>
-      <c r="C482" s="7"/>
+      <c r="B482" s="29"/>
+      <c r="C482" s="30"/>
       <c r="D482" s="7"/>
       <c r="E482" s="7"/>
-      <c r="F482" s="7"/>
+      <c r="F482" s="29"/>
       <c r="G482" s="30"/>
       <c r="H482" s="7"/>
     </row>
@@ -12303,11 +12407,24 @@
       <c r="G872" s="30"/>
       <c r="H872" s="7"/>
     </row>
+    <row r="873" spans="1:8">
+      <c r="A873" s="7"/>
+      <c r="B873" s="7"/>
+      <c r="C873" s="7"/>
+      <c r="D873" s="7"/>
+      <c r="E873" s="7"/>
+      <c r="F873" s="7"/>
+      <c r="G873" s="30"/>
+      <c r="H873" s="7"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="69" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="G57:G59 G52:G53" formulaRange="1"/>
+  </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>